<commit_message>
Apollo 10 Rendezvous Checklists
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 10" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -60,9 +60,6 @@
     <t>SM Fuel Total</t>
   </si>
   <si>
-    <t>CM Fuel Total</t>
-  </si>
-  <si>
     <t>SM Empty Mass</t>
   </si>
   <si>
@@ -136,6 +133,21 @@
   </si>
   <si>
     <t>SLA</t>
+  </si>
+  <si>
+    <t>Total Ascent Stage Mass</t>
+  </si>
+  <si>
+    <t>Total Descent Stage Mass</t>
+  </si>
+  <si>
+    <t>LM Crew/Equip</t>
+  </si>
+  <si>
+    <t>CSM Total Mass</t>
+  </si>
+  <si>
+    <t>CM Total Mass</t>
   </si>
 </sst>
 </file>
@@ -487,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,10 +532,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -540,19 +552,19 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>43.9</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C23" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
+        <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
         <v>19.912705043000003</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>44.1</v>
@@ -564,7 +576,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>78.3</v>
@@ -576,7 +588,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>78.2</v>
@@ -588,56 +600,63 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>B3+B4+B5+B6</f>
+        <v>244.5</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>110.903334465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B9">
+        <v>10700</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4853.4383589999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>10700</v>
+        <v>15709</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>4853.4383589999998</v>
+        <v>7125.4825403300001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>15709</v>
+        <v>25097</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>7125.4825403300001</v>
+        <v>11383.807709890001</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>25097</v>
+        <v>109.9</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>11383.807709890001</v>
+        <v>49.849801463000006</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -645,11 +664,11 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>109.9</v>
+        <v>109.4</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>49.849801463000006</v>
+        <v>49.623005278000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,11 +700,11 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>109.4</v>
+        <v>226.9</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>49.623005278000001</v>
+        <v>102.92010875300001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,11 +712,11 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>226.9</v>
+        <v>224.9</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>102.92010875300001</v>
+        <v>102.01292401300002</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,11 +724,11 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>224.9</v>
+        <v>225.7</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>102.01292401300002</v>
+        <v>102.375797909</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,147 +736,157 @@
         <v>33</v>
       </c>
       <c r="B19">
-        <v>225.7</v>
+        <v>225.3</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>102.375797909</v>
+        <v>102.19436096100002</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B20">
-        <v>225.3</v>
+        <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
+        <v>1340.8999999999999</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>102.19436096100002</v>
+        <v>608.22200893299987</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B10+B11</f>
+        <v>40806</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24">
+        <v>18509.290250220001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
         <v>23098</v>
       </c>
-      <c r="C24">
-        <f>(CONVERT(B24,"lbm","g"))/1000</f>
+      <c r="C23">
+        <f>(CONVERT(B23,"lbm","g"))/1000</f>
         <v>10477.076562259999</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>4703</v>
+      </c>
       <c r="C25">
-        <f t="shared" ref="C25:C41" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>0</v>
+        <f t="shared" ref="C25" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2133.2449161100003</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>4703</v>
+        <v>7009.5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C40" si="2">(CONVERT(B26,"lbm","g"))/1000</f>
+        <v>3179.4557175150003</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>7009.5</v>
+        <v>11209.2</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
-        <v>3179.4557175150003</v>
+        <f t="shared" si="2"/>
+        <v>5084.4075938040005</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>11209.2</v>
+        <f>B26+B27</f>
+        <v>18218.7</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>5084.4075938040005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8263.8633113190008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>5393</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>2446.22365141</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>5393</v>
+        <v>981</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>2446.22365141</v>
+        <f t="shared" si="2"/>
+        <v>444.97411497000002</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32">
-        <v>981</v>
+        <v>1650</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>444.97411497000002</v>
+        <f t="shared" si="2"/>
+        <v>748.42741049999995</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B33">
-        <v>1650</v>
+        <v>108</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>748.42741049999995</v>
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B34">
         <v>108</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48.98797596</v>
       </c>
     </row>
@@ -866,11 +895,11 @@
         <v>19</v>
       </c>
       <c r="B35">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
-        <v>48.98797596</v>
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,7 +910,7 @@
         <v>209</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.800805330000003</v>
       </c>
     </row>
@@ -890,40 +919,36 @@
         <v>21</v>
       </c>
       <c r="B37">
-        <v>209</v>
+        <f>B33+B34+B35+B36</f>
+        <v>634</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>94.800805330000003</v>
+        <f t="shared" si="2"/>
+        <v>287.57756258000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f>B31+B32</f>
+        <v>2631</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>1193.40152547</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40">
         <v>4000</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="1"/>
+      <c r="C40">
+        <f t="shared" si="2"/>
         <v>1814.3694800000001</v>
       </c>
     </row>
@@ -935,15 +960,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
@@ -968,391 +993,219 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>12319</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>0</v>
+        <v>5587.8044060299999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>44.2</v>
+        <f>B2-B4</f>
+        <v>12049</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C39" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>20.048782754000005</v>
+        <f>(CONVERT(B3,"lbm","g"))/1000</f>
+        <v>5465.3344661300007</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>44.2</v>
+        <v>270</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>20.048782754000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5">
-        <v>78.3</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>35.516282571000005</v>
+        <f t="shared" ref="C4:C20" si="0">(CONVERT(B4,"lbm","g"))/1000</f>
+        <v>122.4699399</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B6">
-        <v>78.3</v>
+        <v>58962</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>35.516282571000005</v>
+        <f>(CONVERT(B6,"lbm","g"))/1000</f>
+        <v>26744.713319940001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <f>B6-B9-B10</f>
+        <v>21629.599999999999</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>(CONVERT(B7,"lbm","g"))/1000</f>
+        <v>9811.0215261520007</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="B8">
+        <f>B6-B2-B9-B10</f>
+        <v>9310.5999999999985</v>
+      </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4223.2171201219999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>1362.4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>617.97424488800004</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>35970</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>13882</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>6296.7692803400005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>22226</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>10081.54401562</v>
+        <v>16315.7175489</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B13">
-        <v>109.8</v>
+        <v>22193</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>49.804442225999999</v>
+        <f t="shared" ref="C13" si="1">(CONVERT(B13,"lbm","g"))/1000</f>
+        <v>10066.575467410001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>109.3</v>
+        <f>B13-B15</f>
+        <v>4249</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>49.577646041000001</v>
+        <v>1927.3139801300001</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>111</v>
+        <v>17944</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>50.348753070000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16">
-        <v>110.6</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>50.167316121999995</v>
+        <v>8139.2614872800004</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B17">
-        <v>223.1</v>
+        <v>9807</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>101.19645774700001</v>
+        <f t="shared" ref="C17" si="2">(CONVERT(B17,"lbm","g"))/1000</f>
+        <v>4448.3803725899998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>225.4</v>
+        <f>B17-B19-B20+B21</f>
+        <v>5476.8</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>102.23972019800001</v>
+        <v>2484.2346920160003</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>226.2</v>
+        <v>4136</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>102.602594094</v>
+        <v>1876.0580423199999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>225.2</v>
+        <v>633</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>102.149001724</v>
+        <v>287.12397020999998</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>438.8</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <f t="shared" ref="C21" si="3">(CONVERT(B21,"lbm","g"))/1000</f>
+        <v>199.036331956</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27">
-        <v>6977</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>3164.7139654900002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28">
-        <v>11063</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>5018.0923893100007</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>1626</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>737.54119362000006</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33">
-        <v>2524</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>1144.86714188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>108</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>48.98797596</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35">
-        <v>108</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>48.98797596</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36">
-        <v>209</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>94.800805330000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37">
-        <v>209</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="0"/>
-        <v>94.800805330000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41">
-        <f t="shared" ref="C41" si="1">(CONVERT(B41,"lbm","g"))/1000</f>
-        <v>0</v>
+      <c r="B23">
+        <v>4002</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23" si="4">(CONVERT(B23,"lbm","g"))/1000</f>
+        <v>1815.2766647400001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apollo 9 & 10 LM Masses
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project Apollo 16\Doc\Project Apollo - NASSP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="Apollo 10" sheetId="6" r:id="rId1"/>
-    <sheet name="Apollo 9" sheetId="3" r:id="rId2"/>
+    <sheet name="Apollo 11" sheetId="7" r:id="rId1"/>
+    <sheet name="Apollo 10" sheetId="6" r:id="rId2"/>
+    <sheet name="Apollo 9" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -153,7 +149,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,7 +498,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,60 +538,45 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>12300</v>
-      </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5579.1861510000008</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3">
-        <v>43.9</v>
-      </c>
       <c r="C3">
         <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>19.912705043000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4">
-        <v>44.1</v>
-      </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>20.003423517000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5">
-        <v>78.3</v>
-      </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>35.516282571000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6">
-        <v>78.2</v>
-      </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>35.470923333999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,143 +585,110 @@
       </c>
       <c r="B7">
         <f>B3+B4+B5+B6</f>
-        <v>244.5</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>110.903334465</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>10700</v>
-      </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4853.4383589999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10">
-        <v>15709</v>
-      </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>7125.4825403300001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>25097</v>
-      </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>11383.807709890001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12">
-        <v>109.9</v>
-      </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>49.849801463000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13">
-        <v>109.4</v>
-      </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>49.623005278000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14">
-        <v>109.4</v>
-      </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>49.623005278000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
-        <v>109.4</v>
-      </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>49.623005278000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16">
-        <v>226.9</v>
-      </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>102.92010875300001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17">
-        <v>224.9</v>
-      </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>102.01292401300002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18">
-        <v>225.7</v>
-      </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>102.375797909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19">
-        <v>225.3</v>
-      </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>102.19436096100002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -749,11 +697,11 @@
       </c>
       <c r="B20">
         <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
-        <v>1340.8999999999999</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>608.22200893299987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,59 +710,47 @@
       </c>
       <c r="B21">
         <f>B10+B11</f>
-        <v>40806</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>18509.290250220001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23">
-        <v>23098</v>
-      </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10477.076562259999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B25">
-        <v>4703</v>
-      </c>
       <c r="C25">
-        <f t="shared" ref="C25" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>2133.2449161100003</v>
+        <f t="shared" ref="C25:C40" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26">
-        <v>7009.5</v>
-      </c>
       <c r="C26">
-        <f t="shared" ref="C26:C40" si="2">(CONVERT(B26,"lbm","g"))/1000</f>
-        <v>3179.4557175150003</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27">
-        <v>11209.2</v>
-      </c>
       <c r="C27">
-        <f t="shared" si="2"/>
-        <v>5084.4075938040005</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,95 +759,74 @@
       </c>
       <c r="B28">
         <f>B26+B27</f>
-        <v>18218.7</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
-        <v>8263.8633113190008</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30">
-        <v>5393</v>
-      </c>
       <c r="C30">
-        <f t="shared" si="2"/>
-        <v>2446.22365141</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B31">
-        <v>981</v>
-      </c>
       <c r="C31">
-        <f t="shared" si="2"/>
-        <v>444.97411497000002</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
-      <c r="B32">
-        <v>1650</v>
-      </c>
       <c r="C32">
-        <f t="shared" si="2"/>
-        <v>748.42741049999995</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
-      <c r="B33">
-        <v>108</v>
-      </c>
       <c r="C33">
-        <f t="shared" si="2"/>
-        <v>48.98797596</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
-      <c r="B34">
-        <v>108</v>
-      </c>
       <c r="C34">
-        <f t="shared" si="2"/>
-        <v>48.98797596</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B35">
-        <v>209</v>
-      </c>
       <c r="C35">
-        <f t="shared" si="2"/>
-        <v>94.800805330000003</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
-      <c r="B36">
-        <v>209</v>
-      </c>
       <c r="C36">
-        <f t="shared" si="2"/>
-        <v>94.800805330000003</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,11 +835,11 @@
       </c>
       <c r="B37">
         <f>B33+B34+B35+B36</f>
-        <v>634</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
-        <v>287.57756258000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -933,23 +848,20 @@
       </c>
       <c r="B38">
         <f>B31+B32</f>
-        <v>2631</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
-        <v>1193.40152547</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="B40">
-        <v>4000</v>
-      </c>
       <c r="C40">
-        <f t="shared" si="2"/>
-        <v>1814.3694800000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -960,10 +872,471 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" customWidth="1"/>
+    <col min="45" max="45" width="20.5703125" customWidth="1"/>
+    <col min="46" max="46" width="17.28515625" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" customWidth="1"/>
+    <col min="54" max="54" width="17.28515625" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>12300</v>
+      </c>
+      <c r="C2">
+        <f>(CONVERT(B2,"lbm","g"))/1000</f>
+        <v>5579.1861510000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>43.9</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
+        <v>19.912705043000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>44.1</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>20.003423517000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>78.3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>35.516282571000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>78.2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>35.470923333999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>B3+B4+B5+B6</f>
+        <v>244.5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>110.903334465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>10700</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4853.4383589999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>15709</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7125.4825403300001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>25097</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>11383.807709890001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>109.9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>49.849801463000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>109.4</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>49.623005278000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>109.4</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>49.623005278000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>109.4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>49.623005278000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>226.9</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>102.92010875300001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>224.9</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>102.01292401300002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>225.7</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>102.375797909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>225.3</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>102.19436096100002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
+        <v>1340.8999999999999</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>608.22200893299987</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B10+B11</f>
+        <v>40806</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>18509.290250220001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>23098</v>
+      </c>
+      <c r="C23">
+        <f>(CONVERT(B23,"lbm","g"))/1000</f>
+        <v>10477.076562259999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>4703</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2133.2449161100003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>7009.5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C40" si="2">(CONVERT(B26,"lbm","g"))/1000</f>
+        <v>3179.4557175150003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>11209.2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>5084.4075938040005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <f>B26+B27</f>
+        <v>18218.7</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>8263.8633113190008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>5393</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>2446.22365141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>981</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>444.97411497000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>1650</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>748.42741049999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>108</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>209</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>209</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <f>B33+B34+B35+B36</f>
+        <v>634</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>287.57756258000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f>B31+B32</f>
+        <v>2631</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>1193.40152547</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <v>4000</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>1814.3694800000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1405,7 @@
         <v>270</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C20" si="0">(CONVERT(B4,"lbm","g"))/1000</f>
+        <f t="shared" ref="C4:C19" si="0">(CONVERT(B4,"lbm","g"))/1000</f>
         <v>122.4699399</v>
       </c>
     </row>
@@ -1098,113 +1471,113 @@
         <v>16315.7175489</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>22193</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12" si="1">(CONVERT(B12,"lbm","g"))/1000</f>
+        <v>10066.575467410001</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>22193</v>
+        <f>B12-B14</f>
+        <v>4249</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13" si="1">(CONVERT(B13,"lbm","g"))/1000</f>
-        <v>10066.575467410001</v>
+        <f t="shared" si="0"/>
+        <v>1927.3139801300001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <f>B13-B15</f>
-        <v>4249</v>
+        <v>17944</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>1927.3139801300001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>17944</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
         <v>8139.2614872800004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>9807</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16" si="2">(CONVERT(B16,"lbm","g"))/1000</f>
+        <v>4448.3803725899998</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>9807</v>
+        <f>B16-B18-B19+B20</f>
+        <v>5476.8</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17" si="2">(CONVERT(B17,"lbm","g"))/1000</f>
-        <v>4448.3803725899998</v>
+        <f t="shared" si="0"/>
+        <v>2484.2346920160003</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <f>B17-B19-B20+B21</f>
-        <v>5476.8</v>
+        <v>4136</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>2484.2346920160003</v>
+        <v>1876.0580423199999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>4136</v>
+        <v>633</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1876.0580423199999</v>
+        <v>287.12397020999998</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B20">
-        <v>633</v>
+        <v>438.8</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>287.12397020999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21">
-        <v>438.8</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ref="C21" si="3">(CONVERT(B21,"lbm","g"))/1000</f>
+        <f t="shared" ref="C20" si="3">(CONVERT(B20,"lbm","g"))/1000</f>
         <v>199.036331956</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B23">
+      <c r="B22">
         <v>4002</v>
       </c>
-      <c r="C23">
-        <f t="shared" ref="C23" si="4">(CONVERT(B23,"lbm","g"))/1000</f>
+      <c r="C22">
+        <f t="shared" ref="C22" si="4">(CONVERT(B22,"lbm","g"))/1000</f>
         <v>1815.2766647400001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Apollo 11 Checklist Fixes (DOI-PDI)
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project Apollo 16\Doc\Project Apollo - NASSP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 11" sheetId="7" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Apollo 9" sheetId="3" r:id="rId3"/>
     <sheet name="Apollo 8" sheetId="10" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -192,7 +197,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +663,7 @@
     <col min="62" max="62" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -666,7 +671,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -688,7 +693,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -709,8 +714,16 @@
       <c r="G3" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>F2+F3+F4+F5</f>
+        <v>14836.552830330002</v>
+      </c>
+      <c r="J3">
+        <f>I3*2.20462</f>
+        <v>32708.961100802124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -732,7 +745,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -754,7 +767,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -766,7 +779,7 @@
         <v>35.516282571000005</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -789,7 +802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
         <v>49</v>
       </c>
@@ -801,7 +814,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -823,7 +836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -845,7 +858,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -857,7 +870,7 @@
         <v>11381.08615567</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -869,7 +882,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -881,7 +894,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -893,7 +906,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -905,7 +918,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2052,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Apollo 11 LM Mass Fixes, Add DEDA commands to Apollo 9
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project Apollo 16\Doc\Project Apollo - NASSP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965"/>
   </bookViews>
@@ -17,7 +12,7 @@
     <sheet name="Apollo 9" sheetId="3" r:id="rId3"/>
     <sheet name="Apollo 8" sheetId="10" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="62">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -192,12 +187,33 @@
   </si>
   <si>
     <t>Default CM RCS</t>
+  </si>
+  <si>
+    <t>LM Launch Mass</t>
+  </si>
+  <si>
+    <t>LM Lunar LO Mass</t>
+  </si>
+  <si>
+    <t>LM Lunar LO RCS</t>
+  </si>
+  <si>
+    <t>LM Descent Empty Calculation</t>
+  </si>
+  <si>
+    <t>LM Ascent Empty Calculation</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>Data From Apollo 11 SCOT &amp; Apollo 11 Mission Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,12 +223,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -307,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -318,6 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,18 +655,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" customWidth="1"/>
@@ -663,7 +686,7 @@
     <col min="62" max="62" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -671,29 +694,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12250</v>
+        <v>12280</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5556.5065325000005</v>
+        <v>5570.1143036000003</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
-        <v>8248.1236560800007</v>
+        <v>8248.2143745540016</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>CONVERT((F2*1000),"g","lbm")</f>
+        <v>18184.200000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -709,21 +736,17 @@
       </c>
       <c r="F3" s="5">
         <f>C38</f>
-        <v>2375.9168340600004</v>
+        <v>2376.0982710079998</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>45</v>
       </c>
       <c r="I3">
-        <f>F2+F3+F4+F5</f>
-        <v>14836.552830330002</v>
-      </c>
-      <c r="J3">
-        <f>I3*2.20462</f>
-        <v>32708.961100802124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
+        <v>5238.3999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -739,13 +762,17 @@
       </c>
       <c r="F4" s="5">
         <f>C25</f>
-        <v>2033.45459471</v>
+        <v>2127.2574968259996</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>4689.7999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -761,13 +788,17 @@
       </c>
       <c r="F5" s="8">
         <f>C30</f>
-        <v>2179.05774548</v>
+        <v>2301.5730446170001</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5074.0999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -778,8 +809,16 @@
         <f t="shared" si="0"/>
         <v>35.516282571000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f>F2+F3+F4+F5</f>
+        <v>15053.143187005</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>33186.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -796,34 +835,34 @@
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4787.6674653500004</v>
+        <v>4785.8530958700003</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="5">
         <f>C2</f>
-        <v>5556.5065325000005</v>
+        <v>5570.1143036000003</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10555</v>
+        <v>10551</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4787.6674653500004</v>
+        <v>4785.8530958700003</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
@@ -836,7 +875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -858,7 +897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -870,7 +909,7 @@
         <v>11381.08615567</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -882,7 +921,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -894,7 +933,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -906,7 +945,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -917,8 +956,11 @@
         <f t="shared" si="0"/>
         <v>49.895160699999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -930,7 +972,7 @@
         <v>102.05828325</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -942,7 +984,7 @@
         <v>102.05828325</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -954,7 +996,7 @@
         <v>102.05828325</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -966,7 +1008,7 @@
         <v>102.05828325</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -979,7 +1021,7 @@
         <v>607.81377580000003</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -992,102 +1034,164 @@
         <v>18507.929473110002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>22805</v>
+        <v>22831</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10344.173997850001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10355.967399469999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25">
-        <v>4483</v>
+        <f>F26</f>
+        <v>4689.7999999999993</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C40" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>2033.45459471</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C25:C40" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2127.2574968259996</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25">
+        <v>33714</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
+        <v>15292.413162180001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26">
-        <v>6975</v>
+        <v>6974.8</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>3163.8067807500001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3163.7160622760002</v>
+      </c>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26">
+        <f>F25-(F30+B28)</f>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26" si="4">(CONVERT(F26,"lbm","g"))/1000</f>
+        <v>2127.2574968259996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>11209</v>
+        <v>11209.4</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
-        <v>5084.3168753300006</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5084.4983122779995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28">
         <f>B26+B27</f>
-        <v>18184</v>
+        <v>18184.2</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>8248.1236560800007</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>8248.2143745540016</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30">
-        <v>4804</v>
+        <f>F31</f>
+        <v>5074.1000000000004</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>2179.05774548</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2301.5730446170001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30">
+        <v>10840</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G32" si="5">(CONVERT(F30,"lbm","g"))/1000</f>
+        <v>4916.9412908000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31">
-        <v>2020</v>
+        <v>2019.9</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>916.25658740000006</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>916.2112281630001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31">
+        <f>F30-(B38+F32)</f>
+        <v>5074.1000000000004</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>2301.5730446170001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
       <c r="B32">
-        <v>3218</v>
+        <v>3218.5</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>1459.66024666</v>
+        <f t="shared" si="2"/>
+        <v>1459.887042845</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32">
+        <v>527.5</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>239.26997517500001</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1098,7 +1202,7 @@
         <v>108</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48.98797596</v>
       </c>
     </row>
@@ -1110,7 +1214,7 @@
         <v>108</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48.98797596</v>
       </c>
     </row>
@@ -1122,7 +1226,7 @@
         <v>209</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.800805330000003</v>
       </c>
     </row>
@@ -1134,7 +1238,7 @@
         <v>209</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.800805330000003</v>
       </c>
     </row>
@@ -1147,7 +1251,7 @@
         <v>634</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>287.57756258000001</v>
       </c>
     </row>
@@ -1157,11 +1261,11 @@
       </c>
       <c r="B38">
         <f>B31+B32</f>
-        <v>5238</v>
+        <v>5238.3999999999996</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>2375.9168340600004</v>
+        <f t="shared" si="2"/>
+        <v>2376.0982710079998</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1169,7 +1273,7 @@
         <v>35</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add saturn masses for Apollo 12 & 13, SC masses for Apollo 12
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FDE57D-F931-46E1-832B-3A54C0F39946}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Apollo 11" sheetId="7" r:id="rId1"/>
-    <sheet name="Apollo 10" sheetId="6" r:id="rId2"/>
-    <sheet name="Apollo 9" sheetId="3" r:id="rId3"/>
-    <sheet name="Apollo 8" sheetId="10" r:id="rId4"/>
+    <sheet name="Apollo 12" sheetId="11" r:id="rId1"/>
+    <sheet name="Apollo 11" sheetId="7" r:id="rId2"/>
+    <sheet name="Apollo 10" sheetId="6" r:id="rId3"/>
+    <sheet name="Apollo 9" sheetId="3" r:id="rId4"/>
+    <sheet name="Apollo 8" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="70">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -147,18 +154,6 @@
     <t>CM Total Mass</t>
   </si>
   <si>
-    <t xml:space="preserve">  DSCFUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ASCFUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  DSCEMPTYMASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ASCEMPTYMASS</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -217,12 +212,39 @@
   </si>
   <si>
     <t>Data From Apollo 8 SCOT &amp; Apollo 8 Mission Report</t>
+  </si>
+  <si>
+    <t>LMDSCFUEL</t>
+  </si>
+  <si>
+    <t>LMASCFUEL</t>
+  </si>
+  <si>
+    <t>LMDSCEMPTY</t>
+  </si>
+  <si>
+    <t>LMASCEMPTY</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>*Assumed same as Apollo 10</t>
+  </si>
+  <si>
+    <t>Data From Apollo 12 Mission Report</t>
+  </si>
+  <si>
+    <t>CSM at SEP</t>
+  </si>
+  <si>
+    <t>LM at SEP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -350,6 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,18 +679,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DAF9E-BC71-4638-95FD-6BF28D732C5B}">
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +718,7 @@
     <col min="62" max="62" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -703,234 +726,252 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12280</v>
+        <v>12283.5</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5570.1143036000003</v>
+        <v>5571.7018768950002</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
-        <v>8248.2143745540016</v>
+        <v>8359.2537867300016</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I2">
         <f>CONVERT((F2*1000),"g","lbm")</f>
-        <v>18184.200000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18429.000000000004</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3">
-        <v>44.8</v>
+        <v>40.6</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>20.320938175999999</v>
+        <v>18.415850222</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F3" s="5">
         <f>C38</f>
-        <v>2376.0982710079998</v>
+        <v>2375.0096493200003</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
-        <v>5238.3999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5236.0000000000009</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4">
-        <v>44.4</v>
+        <v>40.6</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>20.139501228</v>
+        <v>18.415850222</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F4" s="5">
         <f>C25</f>
-        <v>2127.2574968259996</v>
+        <v>2163.680964137</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>4689.7999999999993</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4770.0999999999995</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5">
-        <v>78.400000000000006</v>
+        <v>63.6</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>35.561641807999997</v>
+        <v>28.848474732000003</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F5" s="8">
         <f>C30</f>
-        <v>2301.5730446170001</v>
+        <v>2525.6023161600001</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>5074.0999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5568</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6">
-        <v>78.3</v>
+        <v>63.6</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>35.516282571000005</v>
+        <v>28.848474732000003</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
-        <v>15053.143187005</v>
+        <v>15423.546716347002</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>33186.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34003.1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
         <f>B3+B4+B5+B6</f>
-        <v>245.89999999999998</v>
+        <v>208.4</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>111.53836378299999</v>
+        <v>94.528649908000006</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4785.8530958700003</v>
+        <v>4638.7530902790004</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="F8" s="5">
         <f>C2</f>
-        <v>5570.1143036000003</v>
+        <v>5571.7018768950002</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10551</v>
+        <v>10226.700000000001</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4785.8530958700003</v>
+        <v>4638.7530902790004</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5">
         <f>C21</f>
-        <v>18507.929473110002</v>
+        <v>18514.279766290001</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>15712</v>
+        <v>15728</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>7126.8433174400006</v>
+        <v>7134.1007953600001</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10" s="8">
         <f>C7</f>
-        <v>111.53836378299999</v>
+        <v>94.528649908000006</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11">
-        <v>25091</v>
+        <v>25089</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>11381.08615567</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11380.178970930001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>49.895160699999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50.348753070000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -942,7 +983,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -954,7 +995,7 @@
         <v>49.895160699999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -966,10 +1007,10 @@
         <v>49.895160699999998</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -998,11 +1039,21 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>102.05828325</v>
+        <v>101.60469088000001</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18">
+        <v>63535.6</v>
+      </c>
+      <c r="G18">
+        <f>F18-(B21+B2+B7)</f>
+        <v>10226.699999999997</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1016,6 +1067,12 @@
         <f t="shared" si="0"/>
         <v>102.05828325</v>
       </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19">
+        <v>33584.199999999997</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1036,11 +1093,11 @@
       </c>
       <c r="B21">
         <f>B10+B11</f>
-        <v>40803</v>
+        <v>40817</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>18507.929473110002</v>
+        <v>18514.279766290001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1049,19 +1106,11 @@
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>22831</v>
+        <v>22510.2</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10355.967399469999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G24" t="s">
-        <v>45</v>
+        <v>10210.454967174001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1069,22 +1118,11 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <f>F26</f>
-        <v>4689.7999999999993</v>
+        <v>4770.1000000000004</v>
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C40" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>2127.2574968259996</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25">
-        <v>33714</v>
-      </c>
-      <c r="G25">
-        <f t="shared" ref="G25" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
-        <v>15292.413162180001</v>
+        <v>2163.680964137</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1092,22 +1130,11 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>6974.8</v>
+        <v>7079</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>3163.7160622760002</v>
-      </c>
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26">
-        <f>F25-(F30+B28)</f>
-        <v>4689.7999999999993</v>
-      </c>
-      <c r="G26">
-        <f t="shared" ref="G26" si="4">(CONVERT(F26,"lbm","g"))/1000</f>
-        <v>2127.2574968259996</v>
+        <v>3210.9803872299999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1115,11 +1142,11 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <v>11209.4</v>
+        <v>11350</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
-        <v>5084.4983122779995</v>
+        <v>5148.2733994999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1128,11 +1155,11 @@
       </c>
       <c r="B28">
         <f>B26+B27</f>
-        <v>18184.2</v>
+        <v>18429</v>
       </c>
       <c r="C28">
         <f t="shared" si="2"/>
-        <v>8248.2143745540016</v>
+        <v>8359.2537867300016</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1140,22 +1167,11 @@
         <v>12</v>
       </c>
       <c r="B30">
-        <f>F31</f>
-        <v>5074.1000000000004</v>
+        <v>5568</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>2301.5730446170001</v>
-      </c>
-      <c r="E30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30">
-        <v>10840</v>
-      </c>
-      <c r="G30">
-        <f t="shared" ref="G30:G32" si="5">(CONVERT(F30,"lbm","g"))/1000</f>
-        <v>4916.9412908000004</v>
+        <v>2525.6023161600001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1163,22 +1179,11 @@
         <v>6</v>
       </c>
       <c r="B31">
-        <v>2019.9</v>
+        <v>2012</v>
       </c>
       <c r="C31">
         <f t="shared" si="2"/>
-        <v>916.2112281630001</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31">
-        <f>F30-(B38+F32)</f>
-        <v>5074.1000000000004</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="5"/>
-        <v>2301.5730446170001</v>
+        <v>912.62784844000009</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1186,24 +1191,14 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <v>3218.5</v>
+        <v>3224</v>
       </c>
       <c r="C32">
         <f t="shared" si="2"/>
-        <v>1459.887042845</v>
-      </c>
-      <c r="E32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32">
-        <v>527.5</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="5"/>
-        <v>239.26997517500001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1462.3818008799999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1215,7 +1210,7 @@
         <v>48.98797596</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -1227,7 +1222,7 @@
         <v>48.98797596</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1234,7 @@
         <v>94.800805330000003</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1251,7 +1246,7 @@
         <v>94.800805330000003</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1264,26 +1259,32 @@
         <v>287.57756258000001</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
       <c r="B38">
         <f>B31+B32</f>
-        <v>5238.3999999999996</v>
+        <v>5236</v>
       </c>
       <c r="C38">
         <f t="shared" si="2"/>
-        <v>2376.0982710079998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2375.0096493200003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
+      <c r="B40">
+        <v>4000</v>
+      </c>
       <c r="C40">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="C40" si="3">(CONVERT(B40,"lbm","g"))/1000</f>
+        <v>1814.3694800000001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1293,11 +1294,665 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" customWidth="1"/>
+    <col min="45" max="45" width="20.5703125" customWidth="1"/>
+    <col min="46" max="46" width="17.28515625" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" customWidth="1"/>
+    <col min="54" max="54" width="17.28515625" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>12280</v>
+      </c>
+      <c r="C2">
+        <f>(CONVERT(B2,"lbm","g"))/1000</f>
+        <v>5570.1143036000003</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="2">
+        <f>C28</f>
+        <v>8248.2143745540016</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2">
+        <f>CONVERT((F2*1000),"g","lbm")</f>
+        <v>18184.200000000004</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>44.8</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
+        <v>20.320938175999999</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="5">
+        <f>C38</f>
+        <v>2376.0982710079998</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
+        <v>5238.3999999999996</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>44.4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>20.139501228</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="5">
+        <f>C25</f>
+        <v>2127.2574968259996</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>35.561641807999997</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="8">
+        <f>C30</f>
+        <v>2301.5730446170001</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5074.0999999999995</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>78.3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>35.516282571000005</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <f>F2+F3+F4+F5</f>
+        <v>15053.143187005</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>33186.5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>B3+B4+B5+B6</f>
+        <v>245.89999999999998</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>111.53836378299999</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2">
+        <f>C9</f>
+        <v>4785.8530958700003</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5">
+        <f>C2</f>
+        <v>5570.1143036000003</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>10551</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4785.8530958700003</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="5">
+        <f>C21</f>
+        <v>18507.929473110002</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>15712</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7126.8433174400006</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="8">
+        <f>C7</f>
+        <v>111.53836378299999</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>25091</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>11381.08615567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>110</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>110</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>225</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>225</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>225</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>225</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
+        <v>1340</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>607.81377580000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B10+B11</f>
+        <v>40803</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>18507.929473110002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <f>B2+B9</f>
+        <v>22831</v>
+      </c>
+      <c r="C23">
+        <f>(CONVERT(B23,"lbm","g"))/1000</f>
+        <v>10355.967399469999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <f>F26</f>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C40" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2127.2574968259996</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25">
+        <v>33714</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
+        <v>15292.413162180001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>6974.8</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>3163.7160622760002</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26">
+        <f>F25-(F30+B28)</f>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26" si="4">(CONVERT(F26,"lbm","g"))/1000</f>
+        <v>2127.2574968259996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>11209.4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>5084.4983122779995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <f>B26+B27</f>
+        <v>18184.2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>8248.2143745540016</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <f>F31</f>
+        <v>5074.1000000000004</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>2301.5730446170001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30">
+        <v>10840</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G32" si="5">(CONVERT(F30,"lbm","g"))/1000</f>
+        <v>4916.9412908000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>2019.9</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>916.2112281630001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31">
+        <f>F30-(B38+F32)</f>
+        <v>5074.1000000000004</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>2301.5730446170001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>3218.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>1459.887042845</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32">
+        <v>527.5</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>239.26997517500001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>108</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>209</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>209</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <f>B33+B34+B35+B36</f>
+        <v>634</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>287.57756258000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f>B31+B32</f>
+        <v>5238.3999999999996</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>2376.0982710079998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <v>4000</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40" si="6">(CONVERT(B40,"lbm","g"))/1000</f>
+        <v>1814.3694800000001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,14 +2000,14 @@
         <v>5579.1861510000008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>8263.8633113190008</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1367,14 +2022,14 @@
         <v>19.912705043000003</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F3" s="5">
         <f>C38</f>
         <v>1193.40152547</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1389,14 +2044,14 @@
         <v>20.003423517000002</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F4" s="5">
         <f>C25</f>
         <v>2133.2449161100003</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1411,14 +2066,14 @@
         <v>35.516282571000005</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F5" s="8">
         <f>C30</f>
         <v>2446.22365141</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1446,26 +2101,26 @@
         <v>110.903334465</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4853.4383589999998</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="5">
         <f>C2</f>
         <v>5579.1861510000008</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1480,14 +2135,14 @@
         <v>4853.4383589999998</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5">
         <f>C21</f>
         <v>18509.290250220001</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1502,14 +2157,14 @@
         <v>7125.4825403300001</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10" s="8">
         <f>C7</f>
         <v>110.903334465</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1548,7 +2203,7 @@
         <v>49.623005278000001</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,12 +2494,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,14 +2547,14 @@
         <v>5587.8044060299999</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2">
         <f>C14</f>
         <v>8139.2614872800004</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1915,14 +2570,14 @@
         <v>5465.3344661300007</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F3" s="5">
         <f>C18</f>
         <v>1876.0580423199999</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1937,26 +2592,26 @@
         <v>122.4699399</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F4" s="5">
         <f>C13</f>
         <v>1927.3139801300001</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F5" s="8">
         <f>C17</f>
         <v>2484.2346920160003</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1984,14 +2639,14 @@
         <v>9811.0215261520007</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <f>C8</f>
         <v>4223.2171201219999</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2007,14 +2662,14 @@
         <v>4223.2171201219999</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="5">
         <f>C3</f>
         <v>5465.3344661300007</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2029,14 +2684,14 @@
         <v>617.97424488800004</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5">
         <f>C10</f>
         <v>16315.7175489</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2051,14 +2706,14 @@
         <v>16315.7175489</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10" s="8">
         <f>C4</f>
         <v>122.4699399</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2073,7 +2728,7 @@
         <v>10066.575467410001</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2180,12 +2835,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,14 +2888,14 @@
         <v>5620.9166490400003</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2252,14 +2907,14 @@
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F3" s="5">
         <f>C38</f>
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2271,14 +2926,14 @@
         <v>0</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F4" s="5">
         <f>C25</f>
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2290,14 +2945,14 @@
         <v>0</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F5" s="8">
         <f>C30</f>
         <v>0</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2322,26 +2977,26 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4842.0985497500005</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="5">
         <f>C2</f>
         <v>5620.9166490400003</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2356,14 +3011,14 @@
         <v>4842.0985497500005</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5">
         <f>C21</f>
         <v>18408.139151709998</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2378,19 +3033,19 @@
         <v>18106.04663329</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10" s="8">
         <f>F15</f>
         <v>111</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>666</v>
@@ -2418,13 +3073,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>55.5</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2436,13 +3091,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F14">
         <v>55.5</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2454,14 +3109,14 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F15">
         <f>F13+F14</f>
         <v>111</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2715,7 +3370,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>19900</v>

</xml_diff>

<commit_message>
Add masses for Apollo 12 and 13 to mass spreadsheets and launch scenarios
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FDE57D-F931-46E1-832B-3A54C0F39946}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1008587-A474-4E10-B796-E642F0E32F0E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Apollo 12" sheetId="11" r:id="rId1"/>
-    <sheet name="Apollo 11" sheetId="7" r:id="rId2"/>
-    <sheet name="Apollo 10" sheetId="6" r:id="rId3"/>
-    <sheet name="Apollo 9" sheetId="3" r:id="rId4"/>
-    <sheet name="Apollo 8" sheetId="10" r:id="rId5"/>
+    <sheet name="Apollo 13" sheetId="12" r:id="rId1"/>
+    <sheet name="Apollo 12" sheetId="11" r:id="rId2"/>
+    <sheet name="Apollo 11" sheetId="7" r:id="rId3"/>
+    <sheet name="Apollo 10" sheetId="6" r:id="rId4"/>
+    <sheet name="Apollo 9" sheetId="3" r:id="rId5"/>
+    <sheet name="Apollo 8" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="73">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -239,6 +240,15 @@
   </si>
   <si>
     <t>LM at SEP</t>
+  </si>
+  <si>
+    <t>Data From Apollo 13 Mission Report &amp; SCOT</t>
+  </si>
+  <si>
+    <t>CM at SEP</t>
+  </si>
+  <si>
+    <t>SLA Ring</t>
   </si>
 </sst>
 </file>
@@ -686,11 +696,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DAF9E-BC71-4638-95FD-6BF28D732C5B}">
-  <dimension ref="A1:J40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67D65E4-4F47-4D15-8C66-BD009E2D808A}">
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,25 +741,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12283.5</v>
+        <v>12473.2</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5571.7018768950002</v>
+        <v>5657.7483494840008</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
-        <v>8359.2537867300016</v>
+        <v>8361.7485447649997</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I2">
         <f>CONVERT((F2*1000),"g","lbm")</f>
-        <v>18429.000000000004</v>
+        <v>18434.499999999996</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
@@ -760,25 +770,25 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>40.6</v>
+        <v>44.2</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>18.415850222</v>
+        <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="5">
         <f>C38</f>
-        <v>2375.0096493200003</v>
+        <v>2371.9252212040001</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
-        <v>5236.0000000000009</v>
+        <v>5229.2</v>
       </c>
       <c r="J3" t="s">
         <v>56</v>
@@ -789,25 +799,25 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>40.6</v>
+        <v>44.6</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>18.415850222</v>
+        <v>20.230219702000003</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="5">
         <f>C25</f>
-        <v>2163.680964137</v>
+        <v>2114.1940365700002</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>4770.0999999999995</v>
+        <v>4661</v>
       </c>
       <c r="J4" t="s">
         <v>56</v>
@@ -818,25 +828,25 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>63.6</v>
+        <v>77.8</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>28.848474732000003</v>
+        <v>35.289486386</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="8">
         <f>C30</f>
-        <v>2525.6023161600001</v>
+        <v>2100.4048285220006</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>41</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>5568</v>
+        <v>4630.6000000000013</v>
       </c>
       <c r="J5" t="s">
         <v>56</v>
@@ -847,22 +857,22 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>63.6</v>
+        <v>78.5</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>28.848474732000003</v>
+        <v>35.607001045000004</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
-        <v>15423.546716347002</v>
+        <v>14948.272631061001</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>34003.1</v>
+        <v>32955.300000000003</v>
       </c>
       <c r="J6" t="s">
         <v>56</v>
@@ -874,18 +884,18 @@
       </c>
       <c r="B7">
         <f>B3+B4+B5+B6</f>
-        <v>208.4</v>
+        <v>245.10000000000002</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>94.528649908000006</v>
+        <v>111.17548988700001</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4638.7530902790004</v>
+        <v>4778.3234625279993</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>41</v>
@@ -897,7 +907,7 @@
       </c>
       <c r="F8" s="5">
         <f>C2</f>
-        <v>5571.7018768950002</v>
+        <v>5657.7483494840008</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>41</v>
@@ -908,18 +918,18 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10226.700000000001</v>
+        <v>10534.4</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4638.7530902790004</v>
+        <v>4778.3234625279993</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="5">
         <f>C21</f>
-        <v>18514.279766290001</v>
+        <v>18400.428081419999</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>41</v>
@@ -930,18 +940,18 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>15728</v>
+        <v>15606</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>7134.1007953600001</v>
+        <v>7078.7625262199999</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="8">
         <f>C7</f>
-        <v>94.528649908000006</v>
+        <v>111.17548988700001</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>41</v>
@@ -952,11 +962,11 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>25089</v>
+        <v>24960</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>11380.178970930001</v>
+        <v>11321.665555200001</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -964,11 +974,11 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>111</v>
+        <v>110.4</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>50.348753070000001</v>
+        <v>50.076597648000003</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -976,11 +986,11 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>110</v>
+        <v>109.5</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>49.895160699999998</v>
+        <v>49.668364515</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -988,11 +998,11 @@
         <v>28</v>
       </c>
       <c r="B14">
-        <v>110</v>
+        <v>110.1</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>49.895160699999998</v>
+        <v>49.940519936999998</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1000,14 +1010,14 @@
         <v>29</v>
       </c>
       <c r="B15">
-        <v>110</v>
+        <v>110.1</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>49.895160699999998</v>
+        <v>49.940519936999998</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1015,187 +1025,183 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>225</v>
+        <v>225.6</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>102.05828325</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102.330438672</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17">
-        <v>225</v>
+        <v>225.5</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>102.05828325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102.285079435</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18">
-        <v>224</v>
+        <v>225.4</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>101.60469088000001</v>
+        <v>102.23972019800001</v>
       </c>
       <c r="E18" t="s">
         <v>68</v>
       </c>
       <c r="F18">
-        <v>63535.6</v>
-      </c>
-      <c r="G18">
-        <f>F18-(B21+B2+B7)</f>
-        <v>10226.699999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63720.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19">
-        <v>225</v>
+        <v>226.2</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>102.05828325</v>
+        <v>102.602594094</v>
       </c>
       <c r="E19" t="s">
         <v>69</v>
       </c>
       <c r="F19">
-        <v>33584.199999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33499.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20">
         <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
-        <v>1340</v>
+        <v>1342.8000000000002</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>607.81377580000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>609.08383443600007</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20">
+        <v>12367.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21">
         <f>B10+B11</f>
-        <v>40817</v>
+        <v>40566</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>18514.279766290001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18400.428081419999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23">
-        <f>B2+B9</f>
-        <v>22510.2</v>
+        <v>23105.599999999999</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10210.454967174001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10480.523864272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25">
-        <v>4770.1000000000004</v>
+        <v>4661</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C40" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>2163.680964137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C25:C38" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2114.1940365700002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26">
-        <v>7079</v>
+        <v>7083.6</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>3210.9803872299999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3213.0669121320002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>11350</v>
+        <v>11350.9</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
-        <v>5148.2733994999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5148.6816326329999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28">
         <f>B26+B27</f>
-        <v>18429</v>
+        <v>18434.5</v>
       </c>
       <c r="C28">
         <f t="shared" si="2"/>
-        <v>8359.2537867300016</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8361.7485447649997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30">
-        <v>5568</v>
+        <f>5263.6-B37</f>
+        <v>4630.6000000000004</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>2525.6023161600001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2100.4048285220006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B31">
-        <v>2012</v>
-      </c>
       <c r="C31">
         <f t="shared" si="2"/>
-        <v>912.62784844000009</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
-      <c r="B32">
-        <v>3224</v>
-      </c>
       <c r="C32">
         <f t="shared" si="2"/>
-        <v>1462.3818008799999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,11 +1209,11 @@
         <v>15</v>
       </c>
       <c r="B33">
-        <v>108</v>
+        <v>107.7</v>
       </c>
       <c r="C33">
         <f t="shared" si="2"/>
-        <v>48.98797596</v>
+        <v>48.851898249000008</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,11 +1221,11 @@
         <v>18</v>
       </c>
       <c r="B34">
-        <v>108</v>
+        <v>107.7</v>
       </c>
       <c r="C34">
         <f t="shared" si="2"/>
-        <v>48.98797596</v>
+        <v>48.851898249000008</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,11 +1233,11 @@
         <v>19</v>
       </c>
       <c r="B35">
-        <v>209</v>
+        <v>208.8</v>
       </c>
       <c r="C35">
         <f t="shared" si="2"/>
-        <v>94.800805330000003</v>
+        <v>94.710086856000004</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,11 +1245,11 @@
         <v>20</v>
       </c>
       <c r="B36">
-        <v>209</v>
+        <v>208.8</v>
       </c>
       <c r="C36">
         <f t="shared" si="2"/>
-        <v>94.800805330000003</v>
+        <v>94.710086856000004</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,11 +1258,11 @@
       </c>
       <c r="B37">
         <f>B33+B34+B35+B36</f>
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C37">
         <f t="shared" si="2"/>
-        <v>287.57756258000001</v>
+        <v>287.12397020999998</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1264,12 +1270,11 @@
         <v>8</v>
       </c>
       <c r="B38">
-        <f>B31+B32</f>
-        <v>5236</v>
+        <v>5229.2</v>
       </c>
       <c r="C38">
         <f t="shared" si="2"/>
-        <v>2375.0096493200003</v>
+        <v>2371.9252212040001</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,6 +1290,18 @@
       </c>
       <c r="D40" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ref="C41" si="4">(CONVERT(B41,"lbm","g"))/1000</f>
+        <v>44.452052260000002</v>
       </c>
     </row>
   </sheetData>
@@ -1294,11 +1311,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DAF9E-BC71-4638-95FD-6BF28D732C5B}">
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,25 +1356,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12280</v>
+        <v>12283.5</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5570.1143036000003</v>
+        <v>5571.7018768950002</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
-        <v>8248.2143745540016</v>
+        <v>8359.2537867300016</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I2">
         <f>CONVERT((F2*1000),"g","lbm")</f>
-        <v>18184.200000000004</v>
+        <v>18429.000000000004</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
@@ -1368,25 +1385,25 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>44.8</v>
+        <v>40.6</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>20.320938175999999</v>
+        <v>18.415850222</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="5">
         <f>C38</f>
-        <v>2376.0982710079998</v>
+        <v>2375.0096493200003</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
-        <v>5238.3999999999996</v>
+        <v>5236.0000000000009</v>
       </c>
       <c r="J3" t="s">
         <v>56</v>
@@ -1397,25 +1414,25 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>44.4</v>
+        <v>40.6</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>20.139501228</v>
+        <v>18.415850222</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="5">
         <f>C25</f>
-        <v>2127.2574968259996</v>
+        <v>2163.680964137</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>4689.7999999999993</v>
+        <v>4770.0999999999995</v>
       </c>
       <c r="J4" t="s">
         <v>56</v>
@@ -1426,25 +1443,25 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>78.400000000000006</v>
+        <v>63.6</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>35.561641807999997</v>
+        <v>28.848474732000003</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="8">
         <f>C30</f>
-        <v>2301.5730446170001</v>
+        <v>2335.5924723670005</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>41</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>5074.0999999999995</v>
+        <v>5149.1000000000004</v>
       </c>
       <c r="J5" t="s">
         <v>56</v>
@@ -1455,22 +1472,22 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>78.3</v>
+        <v>63.6</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>35.516282571000005</v>
+        <v>28.848474732000003</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
-        <v>15053.143187005</v>
+        <v>15233.536872554003</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>33186.5</v>
+        <v>33584.200000000004</v>
       </c>
       <c r="J6" t="s">
         <v>56</v>
@@ -1482,18 +1499,18 @@
       </c>
       <c r="B7">
         <f>B3+B4+B5+B6</f>
-        <v>245.89999999999998</v>
+        <v>208.4</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>111.53836378299999</v>
+        <v>94.528649908000006</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4785.8530958700003</v>
+        <v>4638.7530902790004</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>41</v>
@@ -1505,7 +1522,7 @@
       </c>
       <c r="F8" s="5">
         <f>C2</f>
-        <v>5570.1143036000003</v>
+        <v>5571.7018768950002</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>41</v>
@@ -1516,18 +1533,18 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10551</v>
+        <v>10226.700000000001</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4785.8530958700003</v>
+        <v>4638.7530902790004</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="5">
         <f>C21</f>
-        <v>18507.929473110002</v>
+        <v>18514.279766290001</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>41</v>
@@ -1538,18 +1555,18 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>15712</v>
+        <v>15728</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>7126.8433174400006</v>
+        <v>7134.1007953600001</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="8">
         <f>C7</f>
-        <v>111.53836378299999</v>
+        <v>94.528649908000006</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>41</v>
@@ -1560,11 +1577,11 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>25091</v>
+        <v>25089</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>11381.08615567</v>
+        <v>11380.178970930001</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1572,11 +1589,11 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>49.895160699999998</v>
+        <v>50.348753070000001</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1615,7 +1632,7 @@
         <v>49.895160699999998</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1647,11 +1664,21 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>102.05828325</v>
+        <v>101.60469088000001</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18">
+        <v>63535.6</v>
+      </c>
+      <c r="G18">
+        <f>F18-(B21+B2+B7)</f>
+        <v>10226.699999999997</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,6 +1692,12 @@
         <f t="shared" si="0"/>
         <v>102.05828325</v>
       </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19">
+        <v>33584.199999999997</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1685,11 +1718,11 @@
       </c>
       <c r="B21">
         <f>B10+B11</f>
-        <v>40803</v>
+        <v>40817</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>18507.929473110002</v>
+        <v>18514.279766290001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1698,19 +1731,11 @@
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>22831</v>
+        <v>22510.2</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10355.967399469999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" t="s">
-        <v>41</v>
+        <v>10210.454967174001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1718,22 +1743,11 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <f>F26</f>
-        <v>4689.7999999999993</v>
+        <v>4770.1000000000004</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C40" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>2127.2574968259996</v>
-      </c>
-      <c r="E25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25">
-        <v>33714</v>
-      </c>
-      <c r="G25">
-        <f t="shared" ref="G25" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
-        <v>15292.413162180001</v>
+        <f t="shared" ref="C25:C38" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2163.680964137</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1741,22 +1755,11 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>6974.8</v>
+        <v>7079</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>3163.7160622760002</v>
-      </c>
-      <c r="E26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26">
-        <f>F25-(F30+B28)</f>
-        <v>4689.7999999999993</v>
-      </c>
-      <c r="G26">
-        <f t="shared" ref="G26" si="4">(CONVERT(F26,"lbm","g"))/1000</f>
-        <v>2127.2574968259996</v>
+        <v>3210.9803872299999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1764,11 +1767,11 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <v>11209.4</v>
+        <v>11350</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
-        <v>5084.4983122779995</v>
+        <v>5148.2733994999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1777,11 +1780,11 @@
       </c>
       <c r="B28">
         <f>B26+B27</f>
-        <v>18184.2</v>
+        <v>18429</v>
       </c>
       <c r="C28">
         <f t="shared" si="2"/>
-        <v>8248.2143745540016</v>
+        <v>8359.2537867300016</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1789,22 +1792,11 @@
         <v>12</v>
       </c>
       <c r="B30">
-        <f>F31</f>
-        <v>5074.1000000000004</v>
+        <v>5149.1000000000004</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>2301.5730446170001</v>
-      </c>
-      <c r="E30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30">
-        <v>10840</v>
-      </c>
-      <c r="G30">
-        <f t="shared" ref="G30:G32" si="5">(CONVERT(F30,"lbm","g"))/1000</f>
-        <v>4916.9412908000004</v>
+        <v>2335.5924723670005</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,22 +1804,11 @@
         <v>6</v>
       </c>
       <c r="B31">
-        <v>2019.9</v>
+        <v>2012</v>
       </c>
       <c r="C31">
         <f t="shared" si="2"/>
-        <v>916.2112281630001</v>
-      </c>
-      <c r="E31" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31">
-        <f>F30-(B38+F32)</f>
-        <v>5074.1000000000004</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="5"/>
-        <v>2301.5730446170001</v>
+        <v>912.62784844000009</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1835,21 +1816,11 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <v>3218.5</v>
+        <v>3224</v>
       </c>
       <c r="C32">
         <f t="shared" si="2"/>
-        <v>1459.887042845</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32">
-        <v>527.5</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="5"/>
-        <v>239.26997517500001</v>
+        <v>1462.3818008799999</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,11 +1890,11 @@
       </c>
       <c r="B38">
         <f>B31+B32</f>
-        <v>5238.3999999999996</v>
+        <v>5236</v>
       </c>
       <c r="C38">
         <f t="shared" si="2"/>
-        <v>2376.0982710079998</v>
+        <v>2375.0096493200003</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,11 +1905,23 @@
         <v>4000</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40" si="6">(CONVERT(B40,"lbm","g"))/1000</f>
+        <f t="shared" ref="C40:C41" si="3">(CONVERT(B40,"lbm","g"))/1000</f>
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>44.452052260000002</v>
       </c>
     </row>
   </sheetData>
@@ -1948,6 +1931,672 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" customWidth="1"/>
+    <col min="45" max="45" width="20.5703125" customWidth="1"/>
+    <col min="46" max="46" width="17.28515625" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" customWidth="1"/>
+    <col min="54" max="54" width="17.28515625" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>12280</v>
+      </c>
+      <c r="C2">
+        <f>(CONVERT(B2,"lbm","g"))/1000</f>
+        <v>5570.1143036000003</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="2">
+        <f>C28</f>
+        <v>8248.2143745540016</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2">
+        <f>CONVERT((F2*1000),"g","lbm")</f>
+        <v>18184.200000000004</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>44.8</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
+        <v>20.320938175999999</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="5">
+        <f>C38</f>
+        <v>2376.0982710079998</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
+        <v>5238.3999999999996</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>44.4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>20.139501228</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="5">
+        <f>C25</f>
+        <v>2127.2574968259996</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>35.561641807999997</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="8">
+        <f>C30</f>
+        <v>2301.5730446170001</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5074.0999999999995</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>78.3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>35.516282571000005</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <f>F2+F3+F4+F5</f>
+        <v>15053.143187005</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>33186.5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>B3+B4+B5+B6</f>
+        <v>245.89999999999998</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>111.53836378299999</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2">
+        <f>C9</f>
+        <v>4785.8530958700003</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5">
+        <f>C2</f>
+        <v>5570.1143036000003</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>10551</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4785.8530958700003</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="5">
+        <f>C21</f>
+        <v>18507.929473110002</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>15712</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7126.8433174400006</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="8">
+        <f>C7</f>
+        <v>111.53836378299999</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>25091</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>11381.08615567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>110</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>110</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>49.895160699999998</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>225</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>225</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>225</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>225</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>102.05828325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
+        <v>1340</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>607.81377580000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B10+B11</f>
+        <v>40803</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>18507.929473110002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <f>B2+B9</f>
+        <v>22831</v>
+      </c>
+      <c r="C23">
+        <f>(CONVERT(B23,"lbm","g"))/1000</f>
+        <v>10355.967399469999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <f>F26</f>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C38" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>2127.2574968259996</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25">
+        <v>33714</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
+        <v>15292.413162180001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>6974.8</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>3163.7160622760002</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26">
+        <f>F25-(F30+B28)</f>
+        <v>4689.7999999999993</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26" si="4">(CONVERT(F26,"lbm","g"))/1000</f>
+        <v>2127.2574968259996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>11209.4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>5084.4983122779995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <f>B26+B27</f>
+        <v>18184.2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>8248.2143745540016</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <f>F31</f>
+        <v>5074.1000000000004</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>2301.5730446170001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30">
+        <v>10840</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G32" si="5">(CONVERT(F30,"lbm","g"))/1000</f>
+        <v>4916.9412908000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>2019.9</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>916.2112281630001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31">
+        <f>F30-(B38+F32)</f>
+        <v>5074.1000000000004</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>2301.5730446170001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>3218.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>1459.887042845</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32">
+        <v>527.5</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>239.26997517500001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>108</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>209</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>209</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <f>B33+B34+B35+B36</f>
+        <v>634</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>287.57756258000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f>B31+B32</f>
+        <v>5238.3999999999996</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>2376.0982710079998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <v>4000</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40:C41" si="6">(CONVERT(B40,"lbm","g"))/1000</f>
+        <v>1814.3694800000001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="6"/>
+        <v>44.452052260000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
@@ -2494,7 +3143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -2835,7 +3484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update sc mass file
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1008587-A474-4E10-B796-E642F0E32F0E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65A312B-A2F2-479A-9B36-D52A017A366D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 13" sheetId="12" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Apollo 9" sheetId="3" r:id="rId5"/>
     <sheet name="Apollo 8" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="74">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>SLA Ring</t>
+  </si>
+  <si>
+    <t>SMRCSFUELLOAD</t>
   </si>
 </sst>
 </file>
@@ -699,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67D65E4-4F47-4D15-8C66-BD009E2D808A}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,11 +1979,12 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12280</v>
+        <f>12280-B7</f>
+        <v>12034.1</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5570.1143036000003</v>
+        <v>5458.5759398170003</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
@@ -2130,7 +2134,7 @@
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4785.8530958700003</v>
+        <v>4178.03932007</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>41</v>
@@ -2142,7 +2146,7 @@
       </c>
       <c r="F8" s="5">
         <f>C2</f>
-        <v>5570.1143036000003</v>
+        <v>5458.5759398170003</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>41</v>
@@ -2153,11 +2157,12 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10551</v>
+        <f>10551-B20</f>
+        <v>9211</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4785.8530958700003</v>
+        <v>4178.03932007</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>46</v>
@@ -2203,6 +2208,16 @@
         <f t="shared" si="0"/>
         <v>11381.08615567</v>
       </c>
+      <c r="E11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
+        <f>C20</f>
+        <v>607.81377580000003</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2227,6 +2242,20 @@
         <f t="shared" si="0"/>
         <v>49.895160699999998</v>
       </c>
+      <c r="F13">
+        <f>SUM(F7:F11)</f>
+        <v>28863.89687258</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13">
+        <f>CONVERT((F13*1000),"g","lbm")</f>
+        <v>63633.999999999993</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2335,11 +2364,11 @@
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>22831</v>
+        <v>21245.1</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10355.967399469999</v>
+        <v>9636.6152598870012</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2369,7 +2398,7 @@
         <v>33714</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
+        <f t="shared" ref="G25:G26" si="3">(CONVERT(F25,"lbm","g"))/1000</f>
         <v>15292.413162180001</v>
       </c>
     </row>
@@ -2392,7 +2421,7 @@
         <v>4689.7999999999993</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26" si="4">(CONVERT(F26,"lbm","g"))/1000</f>
+        <f t="shared" si="3"/>
         <v>2127.2574968259996</v>
       </c>
     </row>
@@ -2440,7 +2469,7 @@
         <v>10840</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:G32" si="5">(CONVERT(F30,"lbm","g"))/1000</f>
+        <f t="shared" ref="G30:G32" si="4">(CONVERT(F30,"lbm","g"))/1000</f>
         <v>4916.9412908000004</v>
       </c>
     </row>
@@ -2463,7 +2492,7 @@
         <v>5074.1000000000004</v>
       </c>
       <c r="G31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2301.5730446170001</v>
       </c>
     </row>
@@ -2485,7 +2514,7 @@
         <v>527.5</v>
       </c>
       <c r="G32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>239.26997517500001</v>
       </c>
     </row>
@@ -2571,7 +2600,7 @@
         <v>4000</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:C41" si="6">(CONVERT(B40,"lbm","g"))/1000</f>
+        <f t="shared" ref="C40:C41" si="5">(CONVERT(B40,"lbm","g"))/1000</f>
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
@@ -2586,7 +2615,7 @@
         <v>98</v>
       </c>
       <c r="C41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>44.452052260000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated SC masses (added SLA ring and fixed Apollo 9 loads)
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E974A8-39E4-4BB4-86F8-5E1CB27052EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A697F7-0DFA-4E16-8972-410594E91950}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 13" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="76">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>SMRCSFUELLOAD</t>
+  </si>
+  <si>
+    <t>SM SLA Ring</t>
+  </si>
+  <si>
+    <t>*Need to review inert CM mass</t>
   </si>
 </sst>
 </file>
@@ -1937,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,7 +2140,7 @@
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4178.03932007</v>
+        <v>4222.4913723299996</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>41</v>
@@ -2157,12 +2163,12 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <f>10551-B20</f>
-        <v>9211</v>
+        <f>10551-B20+B41</f>
+        <v>9309</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4178.03932007</v>
+        <v>4222.4913723299996</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>46</v>
@@ -2244,14 +2250,14 @@
       </c>
       <c r="F13">
         <f>SUM(F7:F11)</f>
-        <v>28863.89687258</v>
+        <v>28908.34892484</v>
       </c>
       <c r="G13" t="s">
         <v>41</v>
       </c>
       <c r="I13">
         <f>CONVERT((F13*1000),"g","lbm")</f>
-        <v>63633.999999999993</v>
+        <v>63732</v>
       </c>
       <c r="J13" t="s">
         <v>56</v>
@@ -2364,11 +2370,11 @@
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>21245.1</v>
+        <v>21343.1</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>9636.6152598870012</v>
+        <v>9681.067312146999</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2627,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,7 +2789,7 @@
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4853.4383589999998</v>
+        <v>4897.8904112600003</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>41</v>
@@ -2806,11 +2812,12 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10700</v>
+        <f>10700+B41</f>
+        <v>10798</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4853.4383589999998</v>
+        <v>4897.8904112600003</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>46</v>
@@ -2856,6 +2863,16 @@
         <f t="shared" si="0"/>
         <v>11383.807709890001</v>
       </c>
+      <c r="E11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
+        <f>C20</f>
+        <v>608.22200893299987</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2920,7 +2937,7 @@
         <v>102.92010875300001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2932,7 +2949,7 @@
         <v>102.01292401300002</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2943,8 +2960,11 @@
         <f t="shared" si="0"/>
         <v>102.375797909</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2956,7 +2976,7 @@
         <v>102.19436096100002</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2969,7 +2989,7 @@
         <v>608.22200893299987</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2982,20 +3002,20 @@
         <v>18509.290250220001</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>23000</v>
+        <v>23098</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10432.62451</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10477.076562259999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -3007,7 +3027,7 @@
         <v>2133.2449161100003</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -3019,7 +3039,7 @@
         <v>3179.4557175150003</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -3031,7 +3051,7 @@
         <v>5084.4075938040005</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -3044,7 +3064,7 @@
         <v>8263.8633113190008</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3056,7 +3076,7 @@
         <v>2446.22365141</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -3068,7 +3088,7 @@
         <v>444.97411497000002</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3164,6 +3184,18 @@
       <c r="C40">
         <f t="shared" si="2"/>
         <v>1814.3694800000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ref="C41" si="3">(CONVERT(B41,"lbm","g"))/1000</f>
+        <v>44.452052260000002</v>
       </c>
     </row>
   </sheetData>
@@ -3174,7 +3206,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -3215,21 +3247,21 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>12319</v>
+        <v>12074</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5587.8044060299999</v>
+        <v>5476.6742753800008</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="2">
-        <f>C14</f>
-        <v>8139.2614872800004</v>
+        <f>C28</f>
+        <v>8182.8063548</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>41</v>
@@ -3237,22 +3269,21 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <f>B2-B4</f>
-        <v>12049</v>
+        <v>44.2</v>
       </c>
       <c r="C3">
-        <f>(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>5465.3344661300007</v>
+        <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
+        <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="5">
-        <f>C18</f>
-        <v>1876.0580423199999</v>
+        <f>C38</f>
+        <v>1882.4083355</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>41</v>
@@ -3260,33 +3291,43 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>270</v>
+        <v>44.2</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C19" si="0">(CONVERT(B4,"lbm","g"))/1000</f>
-        <v>122.4699399</v>
+        <f t="shared" si="0"/>
+        <v>20.048782754000005</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="5">
-        <f>C13</f>
-        <v>1927.3139801300001</v>
+        <f>C25</f>
+        <v>1883.7691126100001</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>78.3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>35.516282571000005</v>
+      </c>
       <c r="E5" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="8">
-        <f>C17</f>
-        <v>2484.2346920160003</v>
+        <f>C30</f>
+        <v>2278.3944745100002</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>41</v>
@@ -3294,57 +3335,46 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>58962</v>
+        <v>78.3</v>
       </c>
       <c r="C6">
-        <f>(CONVERT(B6,"lbm","g"))/1000</f>
-        <v>26744.713319940001</v>
+        <f t="shared" si="0"/>
+        <v>35.516282571000005</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <f>B6-B9-B10</f>
-        <v>21629.599999999999</v>
+        <f>B3+B4+B5+B6</f>
+        <v>245</v>
       </c>
       <c r="C7">
-        <f>(CONVERT(B7,"lbm","g"))/1000</f>
-        <v>9811.0215261520007</v>
+        <f t="shared" si="0"/>
+        <v>111.13013065000001</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="2">
-        <f>C8</f>
-        <v>4223.2171201219999</v>
+        <f>C9</f>
+        <v>4170.5096867279999</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <f>B6-B2-B9-B10</f>
-        <v>9310.5999999999985</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>4223.2171201219999</v>
-      </c>
       <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="5">
-        <f>C3</f>
-        <v>5465.3344661300007</v>
+        <f>C2</f>
+        <v>5476.6742753800008</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>41</v>
@@ -3352,21 +3382,21 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>1362.4</v>
+        <v>9194.4</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>617.97424488800004</v>
+        <v>4170.5096867279999</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="5">
-        <f>C10</f>
-        <v>16315.7175489</v>
+        <f>C21</f>
+        <v>16378.313295960001</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>41</v>
@@ -3374,136 +3404,712 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>35970</v>
+        <v>13882</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>16315.7175489</v>
+        <v>6296.7692803400005</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="8">
-        <f>C4</f>
-        <v>122.4699399</v>
+        <f>C7</f>
+        <v>111.13013065000001</v>
       </c>
       <c r="G10" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>22226</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10081.54401562</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
+        <f>C20</f>
+        <v>608.085931222</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>22193</v>
+        <v>109.8</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12" si="1">(CONVERT(B12,"lbm","g"))/1000</f>
-        <v>10066.575467410001</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>59</v>
+        <f t="shared" si="0"/>
+        <v>49.804442225999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <f>B12-B14</f>
-        <v>4249</v>
+        <v>109.3</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>1927.3139801300001</v>
+        <v>49.577646041000001</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B14">
-        <v>17944</v>
+        <v>111</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>8139.2614872800004</v>
+        <v>50.348753070000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>110.6</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>50.167316121999995</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>223.1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>101.19645774700001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>225.4</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>102.23972019800001</v>
+      </c>
+      <c r="F17">
+        <v>58962</v>
+      </c>
+      <c r="G17">
+        <f>F17-(B7+B20+B21)</f>
+        <v>21268.400000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>226.2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>102.602594094</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>225.2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>102.149001724</v>
+      </c>
+      <c r="F19">
+        <v>12319</v>
+      </c>
+      <c r="G19">
+        <f>F19-B7</f>
+        <v>12074</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
+        <v>1340.6000000000001</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>608.085931222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B10+B11</f>
+        <v>36108</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>16378.313295960001</v>
+      </c>
+      <c r="F21">
+        <f>G17-G19</f>
+        <v>9194.4000000000015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <f>B2+B9</f>
+        <v>21268.400000000001</v>
+      </c>
+      <c r="C23">
+        <f>(CONVERT(B23,"lbm","g"))/1000</f>
+        <v>9647.1839621080017</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>4153</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C40" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>1883.7691126100001</v>
+      </c>
+      <c r="F25">
+        <v>22193</v>
+      </c>
+      <c r="G25">
+        <f>F25-B28</f>
+        <v>4153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>6977</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>3164.7139654900002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>11063</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>5018.0923893100007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <f>B26+B27</f>
+        <v>18040</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>8182.8063548</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>5023</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>2278.3944745100002</v>
+      </c>
+      <c r="F30">
+        <v>9807</v>
+      </c>
+      <c r="G30">
+        <f>F30-(B38+B37)</f>
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>1626</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>737.54119362000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>2524</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>1144.86714188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>108</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>48.98797596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>209</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>209</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>94.800805330000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <f>B33+B34+B35+B36</f>
+        <v>634</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>287.57756258000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f>B31+B32</f>
+        <v>4150</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>1882.4083355</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <v>4002</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>1815.2766647400001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45">
+        <v>12319</v>
+      </c>
+      <c r="C45">
+        <f>(CONVERT(B45,"lbm","g"))/1000</f>
+        <v>5587.8044060299999</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="2">
+        <f>C59</f>
+        <v>8139.2614872800004</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <f>B45-B47</f>
+        <v>12049</v>
+      </c>
+      <c r="C46">
+        <f>(CONVERT(B46,"lbm","g"))/1000</f>
+        <v>5465.3344661300007</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="5">
+        <f>C63</f>
+        <v>1876.0580423199999</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>270</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:C64" si="2">(CONVERT(B47,"lbm","g"))/1000</f>
+        <v>122.4699399</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="5">
+        <f>C58</f>
+        <v>1927.3139801300001</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="8">
+        <f>C62</f>
+        <v>2484.2346920160003</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49">
+        <v>58962</v>
+      </c>
+      <c r="C49">
+        <f>(CONVERT(B49,"lbm","g"))/1000</f>
+        <v>26744.713319940001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50">
+        <f>B49-B54-B55</f>
+        <v>21629.599999999999</v>
+      </c>
+      <c r="C50">
+        <f>(CONVERT(B50,"lbm","g"))/1000</f>
+        <v>9811.0215261520007</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="2">
+        <f>C53</f>
+        <v>4223.2171201219999</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>15709</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:C52" si="3">(CONVERT(B51,"lbm","g"))/1000</f>
+        <v>7125.4825403300001</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="5">
+        <f>C46</f>
+        <v>5465.3344661300007</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>25097</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>11383.807709890001</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" s="5">
+        <f>C55</f>
+        <v>16315.7175489</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53">
+        <f>B49-B45-B54-B55</f>
+        <v>9310.5999999999985</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>4223.2171201219999</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="8">
+        <f>C47</f>
+        <v>122.4699399</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54">
+        <v>1362.4</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>617.97424488800004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>35970</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>16315.7175489</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57">
+        <v>22193</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57" si="4">(CONVERT(B57,"lbm","g"))/1000</f>
+        <v>10066.575467410001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <f>B57-B59</f>
+        <v>4249</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>1927.3139801300001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <v>17944</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>8139.2614872800004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>36</v>
       </c>
-      <c r="B16">
+      <c r="B61">
         <v>9807</v>
       </c>
-      <c r="C16">
-        <f t="shared" ref="C16" si="2">(CONVERT(B16,"lbm","g"))/1000</f>
+      <c r="C61">
+        <f t="shared" ref="C61" si="5">(CONVERT(B61,"lbm","g"))/1000</f>
         <v>4448.3803725899998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>12</v>
       </c>
-      <c r="B17">
-        <f>B16-B18-B19+B20</f>
+      <c r="B62">
+        <f>B61-B63-B64+B65</f>
         <v>5476.8</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
+      <c r="C62">
+        <f t="shared" si="2"/>
         <v>2484.2346920160003</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>6</v>
       </c>
-      <c r="B18">
+      <c r="B63">
         <v>4136</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
+      <c r="C63">
+        <f t="shared" si="2"/>
         <v>1876.0580423199999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B64">
         <v>633</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
+      <c r="C64">
+        <f t="shared" si="2"/>
         <v>287.12397020999998</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>38</v>
       </c>
-      <c r="B20">
+      <c r="B65">
         <v>438.8</v>
       </c>
-      <c r="C20">
-        <f t="shared" ref="C20" si="3">(CONVERT(B20,"lbm","g"))/1000</f>
+      <c r="C65">
+        <f t="shared" ref="C65" si="6">(CONVERT(B65,"lbm","g"))/1000</f>
         <v>199.036331956</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>35</v>
       </c>
-      <c r="B22">
+      <c r="B67">
         <v>4002</v>
       </c>
-      <c r="C22">
-        <f t="shared" ref="C22" si="4">(CONVERT(B22,"lbm","g"))/1000</f>
+      <c r="C67">
+        <f t="shared" ref="C67" si="7">(CONVERT(B67,"lbm","g"))/1000</f>
         <v>1815.2766647400001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix typo on Apollo 9 mass tab
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A697F7-0DFA-4E16-8972-410594E91950}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC9012B-31F4-422C-8520-20EA6C8D049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="1800" windowWidth="15405" windowHeight="9225" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 13" sheetId="12" r:id="rId1"/>
@@ -20,17 +20,28 @@
     <sheet name="Apollo 9" sheetId="3" r:id="rId5"/>
     <sheet name="Apollo 8" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="72">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -140,21 +151,6 @@
     <t>SLA</t>
   </si>
   <si>
-    <t>Total Ascent Stage Mass</t>
-  </si>
-  <si>
-    <t>Total Descent Stage Mass</t>
-  </si>
-  <si>
-    <t>LM Crew/Equip</t>
-  </si>
-  <si>
-    <t>CSM Total Mass</t>
-  </si>
-  <si>
-    <t>CM Total Mass</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -258,6 +254,9 @@
   </si>
   <si>
     <t>*Need to review inert CM mass</t>
+  </si>
+  <si>
+    <t>LMRCS</t>
   </si>
 </sst>
 </file>
@@ -379,13 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -708,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67D65E4-4F47-4D15-8C66-BD009E2D808A}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -757,21 +755,21 @@
         <v>5657.7483494840008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>8361.7485447649997</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <f>CONVERT((F2*1000),"g","lbm")</f>
         <v>18434.499999999996</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -786,21 +784,21 @@
         <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5">
+        <v>57</v>
+      </c>
+      <c r="F3">
         <f>C38</f>
         <v>2371.9252212040001</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
         <v>5229.2</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -815,21 +813,21 @@
         <v>20.230219702000003</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="F4">
         <f>C25</f>
         <v>2114.1940365700002</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>41</v>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
         <v>4661</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -843,22 +841,22 @@
         <f t="shared" si="0"/>
         <v>35.289486386</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7">
         <f>C30</f>
         <v>2100.4048285220006</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>41</v>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
         <v>4630.6000000000013</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -872,8 +870,8 @@
         <f t="shared" si="0"/>
         <v>35.607001045000004</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>65</v>
+      <c r="E6" t="s">
+        <v>60</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
@@ -884,7 +882,7 @@
         <v>32955.300000000003</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -900,26 +898,26 @@
         <v>111.17548988700001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4778.3234625279993</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <f>C2</f>
         <v>5657.7483494840008</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -934,14 +932,14 @@
         <v>4778.3234625279993</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="5">
+        <v>41</v>
+      </c>
+      <c r="F9">
         <f>C21</f>
         <v>18400.428081419999</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -955,15 +953,15 @@
         <f t="shared" si="0"/>
         <v>7078.7625262199999</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7">
         <f>C7</f>
         <v>111.17548988700001</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>41</v>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1025,8 +1023,8 @@
         <f t="shared" si="0"/>
         <v>49.940519936999998</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>70</v>
+      <c r="E15" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1065,7 +1063,7 @@
         <v>102.23972019800001</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F18">
         <v>63720.3</v>
@@ -1083,7 +1081,7 @@
         <v>102.602594094</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F19">
         <v>33499.1</v>
@@ -1102,7 +1100,7 @@
         <v>609.08383443600007</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F20">
         <v>12367.6</v>
@@ -1298,12 +1296,12 @@
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -1323,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DAF9E-BC71-4638-95FD-6BF28D732C5B}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,21 +1370,21 @@
         <v>5571.7018768950002</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>8359.2537867300016</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <f>CONVERT((F2*1000),"g","lbm")</f>
         <v>18429.000000000004</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1401,21 +1399,21 @@
         <v>18.415850222</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5">
+        <v>57</v>
+      </c>
+      <c r="F3">
         <f>C38</f>
         <v>2375.0096493200003</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
         <v>5236.0000000000009</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1430,21 +1428,21 @@
         <v>18.415850222</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="F4">
         <f>C25</f>
         <v>2163.680964137</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>41</v>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
         <v>4770.0999999999995</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1458,22 +1456,22 @@
         <f t="shared" si="0"/>
         <v>28.848474732000003</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7">
         <f>C30</f>
         <v>2335.5924723670005</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>41</v>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
         <v>5149.1000000000004</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1487,8 +1485,8 @@
         <f t="shared" si="0"/>
         <v>28.848474732000003</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>65</v>
+      <c r="E6" t="s">
+        <v>60</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
@@ -1499,7 +1497,7 @@
         <v>33584.200000000004</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1515,26 +1513,26 @@
         <v>94.528649908000006</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4638.7530902790004</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <f>C2</f>
         <v>5571.7018768950002</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1549,14 +1547,14 @@
         <v>4638.7530902790004</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="5">
+        <v>41</v>
+      </c>
+      <c r="F9">
         <f>C21</f>
         <v>18514.279766290001</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1570,15 +1568,15 @@
         <f t="shared" si="0"/>
         <v>7134.1007953600001</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7">
         <f>C7</f>
         <v>94.528649908000006</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>41</v>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1640,8 +1638,8 @@
         <f t="shared" si="0"/>
         <v>49.895160699999998</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>67</v>
+      <c r="E15" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1680,7 +1678,7 @@
         <v>101.60469088000001</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F18">
         <v>63535.6</v>
@@ -1702,7 +1700,7 @@
         <v>102.05828325</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F19">
         <v>33584.199999999997</v>
@@ -1918,12 +1916,12 @@
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -1993,21 +1991,21 @@
         <v>5458.5759398170003</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>8248.2143745540016</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <f>CONVERT((F2*1000),"g","lbm")</f>
         <v>18184.200000000004</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2022,21 +2020,21 @@
         <v>20.320938175999999</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5">
+        <v>57</v>
+      </c>
+      <c r="F3">
         <f>C38</f>
         <v>2376.0982710079998</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="1">CONVERT((F3*1000),"g","lbm")</f>
         <v>5238.3999999999996</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2051,21 +2049,21 @@
         <v>20.139501228</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="F4">
         <f>C25</f>
         <v>2127.2574968259996</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>41</v>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
         <v>4689.7999999999993</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2079,22 +2077,22 @@
         <f t="shared" si="0"/>
         <v>35.561641807999997</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7">
         <f>C30</f>
         <v>2301.5730446170001</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>41</v>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
         <v>5074.0999999999995</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2108,8 +2106,8 @@
         <f t="shared" si="0"/>
         <v>35.516282571000005</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>65</v>
+      <c r="E6" t="s">
+        <v>60</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
@@ -2120,7 +2118,7 @@
         <v>33186.5</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2136,26 +2134,26 @@
         <v>111.53836378299999</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4222.4913723299996</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <f>C2</f>
         <v>5458.5759398170003</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2171,14 +2169,14 @@
         <v>4222.4913723299996</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="5">
+        <v>41</v>
+      </c>
+      <c r="F9">
         <f>C21</f>
         <v>18507.929473110002</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2192,15 +2190,15 @@
         <f t="shared" si="0"/>
         <v>7126.8433174400006</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7">
         <f>C7</f>
         <v>111.53836378299999</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>41</v>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2214,15 +2212,15 @@
         <f t="shared" si="0"/>
         <v>11381.08615567</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>73</v>
+      <c r="E11" t="s">
+        <v>68</v>
       </c>
       <c r="F11">
         <f>C20</f>
         <v>607.81377580000003</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>41</v>
+      <c r="G11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2253,14 +2251,14 @@
         <v>28908.34892484</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I13">
         <f>CONVERT((F13*1000),"g","lbm")</f>
         <v>63732</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2286,8 +2284,8 @@
         <f t="shared" si="0"/>
         <v>49.895160699999998</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>57</v>
+      <c r="E15" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2379,10 +2377,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2398,7 +2396,7 @@
         <v>2127.2574968259996</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F25">
         <v>33714</v>
@@ -2420,7 +2418,7 @@
         <v>3163.7160622760002</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F26">
         <f>F25-(F30+B28)</f>
@@ -2469,7 +2467,7 @@
         <v>2301.5730446170001</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F30">
         <v>10840</v>
@@ -2491,7 +2489,7 @@
         <v>916.2112281630001</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F31">
         <f>F30-(B38+F32)</f>
@@ -2514,7 +2512,7 @@
         <v>1459.887042845</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F32">
         <v>527.5</v>
@@ -2610,12 +2608,12 @@
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -2635,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,14 +2682,14 @@
         <v>5579.1861510000008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>8263.8633113190008</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2706,14 +2704,14 @@
         <v>19.912705043000003</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5">
+        <v>57</v>
+      </c>
+      <c r="F3">
         <f>C38</f>
         <v>1193.40152547</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2728,14 +2726,14 @@
         <v>20.003423517000002</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="F4">
         <f>C25</f>
         <v>2133.2449161100003</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>41</v>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2749,15 +2747,15 @@
         <f t="shared" si="0"/>
         <v>35.516282571000005</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7">
         <f>C30</f>
         <v>2446.22365141</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>41</v>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2785,26 +2783,26 @@
         <v>110.903334465</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4897.8904112600003</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <f>C2</f>
         <v>5579.1861510000008</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2820,14 +2818,14 @@
         <v>4897.8904112600003</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="5">
+        <v>41</v>
+      </c>
+      <c r="F9">
         <f>C21</f>
         <v>18509.290250220001</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2841,15 +2839,15 @@
         <f t="shared" si="0"/>
         <v>7125.4825403300001</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7">
         <f>C7</f>
         <v>110.903334465</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>41</v>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2863,15 +2861,15 @@
         <f t="shared" si="0"/>
         <v>11383.807709890001</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>73</v>
+      <c r="E11" t="s">
+        <v>68</v>
       </c>
       <c r="F11">
         <f>C20</f>
         <v>608.22200893299987</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>41</v>
+      <c r="G11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2897,8 +2895,8 @@
         <f t="shared" si="0"/>
         <v>49.623005278000001</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>58</v>
+      <c r="E13" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2961,7 +2959,7 @@
         <v>102.375797909</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3188,7 +3186,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -3206,10 +3204,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3237,7 +3235,7 @@
     <col min="62" max="62" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -3245,7 +3243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3257,17 +3255,25 @@
         <v>5476.6742753800008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>8182.8063548</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I2">
+        <f>SUM(F2:F6)</f>
+        <v>14514.955839999999</v>
+      </c>
+      <c r="J2">
+        <f>CONVERT(I2*1000,"g","lbm")</f>
+        <v>31999.999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3279,17 +3285,17 @@
         <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5">
+        <v>57</v>
+      </c>
+      <c r="F3">
         <f>C38</f>
         <v>1882.4083355</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3301,17 +3307,17 @@
         <v>20.048782754000005</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="F4">
         <f>C25</f>
         <v>1883.7691126100001</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3322,18 +3328,18 @@
         <f t="shared" si="0"/>
         <v>35.516282571000005</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7">
         <f>C30</f>
         <v>2278.3944745100002</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3344,8 +3350,18 @@
         <f t="shared" si="0"/>
         <v>35.516282571000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6">
+        <f>C37</f>
+        <v>287.57756258000001</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3358,29 +3374,37 @@
         <v>111.13013065000001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4170.5096867279999</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I7">
+        <f>SUM(F7:F11)</f>
+        <v>26744.713319939998</v>
+      </c>
+      <c r="J7">
+        <f>CONVERT(I7*1000,"g","lbm")</f>
+        <v>58961.999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <f>C2</f>
         <v>5476.6742753800008</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3392,17 +3416,17 @@
         <v>4170.5096867279999</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="5">
+        <v>41</v>
+      </c>
+      <c r="F9">
         <f>C21</f>
         <v>16378.313295960001</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3413,18 +3437,18 @@
         <f t="shared" si="0"/>
         <v>6296.7692803400005</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7">
         <f>C7</f>
         <v>111.13013065000001</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3435,18 +3459,18 @@
         <f t="shared" si="0"/>
         <v>10081.54401562</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>73</v>
+      <c r="E11" t="s">
+        <v>68</v>
       </c>
       <c r="F11">
         <f>C20</f>
         <v>608.085931222</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -3458,7 +3482,7 @@
         <v>49.804442225999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3469,11 +3493,11 @@
         <f t="shared" si="0"/>
         <v>49.577646041000001</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3485,7 +3509,7 @@
         <v>50.348753070000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3497,7 +3521,7 @@
         <v>50.167316121999995</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3701,7 +3725,7 @@
         <v>1144.86714188</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -3713,7 +3737,7 @@
         <v>48.98797596</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3725,7 +3749,7 @@
         <v>48.98797596</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3737,7 +3761,7 @@
         <v>94.800805330000003</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -3749,7 +3773,7 @@
         <v>94.800805330000003</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -3762,7 +3786,7 @@
         <v>287.57756258000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -3775,342 +3799,16 @@
         <v>1882.4083355</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
       <c r="B40">
-        <v>4002</v>
+        <v>3776</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>1815.2766647400001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45">
-        <v>12319</v>
-      </c>
-      <c r="C45">
-        <f>(CONVERT(B45,"lbm","g"))/1000</f>
-        <v>5587.8044060299999</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F45" s="2">
-        <f>C59</f>
-        <v>8139.2614872800004</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46">
-        <f>B45-B47</f>
-        <v>12049</v>
-      </c>
-      <c r="C46">
-        <f>(CONVERT(B46,"lbm","g"))/1000</f>
-        <v>5465.3344661300007</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="5">
-        <f>C63</f>
-        <v>1876.0580423199999</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47">
-        <v>270</v>
-      </c>
-      <c r="C47">
-        <f t="shared" ref="C47:C64" si="2">(CONVERT(B47,"lbm","g"))/1000</f>
-        <v>122.4699399</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F47" s="5">
-        <f>C58</f>
-        <v>1927.3139801300001</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E48" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F48" s="8">
-        <f>C62</f>
-        <v>2484.2346920160003</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49">
-        <v>58962</v>
-      </c>
-      <c r="C49">
-        <f>(CONVERT(B49,"lbm","g"))/1000</f>
-        <v>26744.713319940001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50">
-        <f>B49-B54-B55</f>
-        <v>21629.599999999999</v>
-      </c>
-      <c r="C50">
-        <f>(CONVERT(B50,"lbm","g"))/1000</f>
-        <v>9811.0215261520007</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F50" s="2">
-        <f>C53</f>
-        <v>4223.2171201219999</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51">
-        <v>15709</v>
-      </c>
-      <c r="C51">
-        <f t="shared" ref="C51:C52" si="3">(CONVERT(B51,"lbm","g"))/1000</f>
-        <v>7125.4825403300001</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" s="5">
-        <f>C46</f>
-        <v>5465.3344661300007</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52">
-        <v>25097</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="3"/>
-        <v>11383.807709890001</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F52" s="5">
-        <f>C55</f>
-        <v>16315.7175489</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53">
-        <f>B49-B45-B54-B55</f>
-        <v>9310.5999999999985</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="2"/>
-        <v>4223.2171201219999</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="8">
-        <f>C47</f>
-        <v>122.4699399</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54">
-        <v>1362.4</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="2"/>
-        <v>617.97424488800004</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55">
-        <v>35970</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="2"/>
-        <v>16315.7175489</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57">
-        <v>22193</v>
-      </c>
-      <c r="C57">
-        <f t="shared" ref="C57" si="4">(CONVERT(B57,"lbm","g"))/1000</f>
-        <v>10066.575467410001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58">
-        <f>B57-B59</f>
-        <v>4249</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="2"/>
-        <v>1927.3139801300001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59">
-        <v>17944</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="2"/>
-        <v>8139.2614872800004</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B61">
-        <v>9807</v>
-      </c>
-      <c r="C61">
-        <f t="shared" ref="C61" si="5">(CONVERT(B61,"lbm","g"))/1000</f>
-        <v>4448.3803725899998</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62">
-        <f>B61-B63-B64+B65</f>
-        <v>5476.8</v>
-      </c>
-      <c r="C62">
-        <f t="shared" si="2"/>
-        <v>2484.2346920160003</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63">
-        <v>4136</v>
-      </c>
-      <c r="C63">
-        <f t="shared" si="2"/>
-        <v>1876.0580423199999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>21</v>
-      </c>
-      <c r="B64">
-        <v>633</v>
-      </c>
-      <c r="C64">
-        <f t="shared" si="2"/>
-        <v>287.12397020999998</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>38</v>
-      </c>
-      <c r="B65">
-        <v>438.8</v>
-      </c>
-      <c r="C65">
-        <f t="shared" ref="C65" si="6">(CONVERT(B65,"lbm","g"))/1000</f>
-        <v>199.036331956</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67">
-        <v>4002</v>
-      </c>
-      <c r="C67">
-        <f t="shared" ref="C67" si="7">(CONVERT(B67,"lbm","g"))/1000</f>
-        <v>1815.2766647400001</v>
+        <v>1712.7647891200002</v>
       </c>
     </row>
   </sheetData>
@@ -4123,7 +3821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -4172,14 +3870,14 @@
         <v>5620.9166490400003</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,14 +3889,14 @@
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5">
+        <v>57</v>
+      </c>
+      <c r="F3">
         <f>C38</f>
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>41</v>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4210,14 +3908,14 @@
         <v>0</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="F4">
         <f>C25</f>
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>41</v>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4228,15 +3926,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7">
         <f>C30</f>
         <v>0</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>41</v>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4261,26 +3959,26 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
         <v>4842.0985497500005</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <f>C2</f>
         <v>5620.9166490400003</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4295,14 +3993,14 @@
         <v>4842.0985497500005</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="5">
+        <v>41</v>
+      </c>
+      <c r="F9">
         <f>C21</f>
         <v>18408.139151709998</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>41</v>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4316,20 +4014,20 @@
         <f t="shared" si="0"/>
         <v>18106.04663329</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7">
         <f>F15</f>
         <v>111</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>41</v>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>666</v>
@@ -4357,13 +4055,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F13">
         <v>55.5</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4375,13 +4073,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F14">
         <v>55.5</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4393,14 +4091,14 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F15">
         <f>F13+F14</f>
         <v>111</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4420,8 +4118,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>60</v>
+      <c r="E17" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4654,7 +4352,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B41">
         <v>19900</v>

</xml_diff>

<commit_message>
Update Saturn (through Apollo 17) & Spacecraft Masses (through Apollo 13)
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC9012B-31F4-422C-8520-20EA6C8D049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86109938-3CD7-43DE-9A2B-464642E5B5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="1800" windowWidth="15405" windowHeight="9225" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 13" sheetId="12" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Apollo 10" sheetId="6" r:id="rId4"/>
     <sheet name="Apollo 9" sheetId="3" r:id="rId5"/>
     <sheet name="Apollo 8" sheetId="10" r:id="rId6"/>
+    <sheet name="Apollo 7" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="69">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -157,9 +158,6 @@
     <t>LTAB</t>
   </si>
   <si>
-    <t>SM Fuel (Unusable)</t>
-  </si>
-  <si>
     <t>SMMASS</t>
   </si>
   <si>
@@ -229,21 +227,9 @@
     <t>*Assumed same as Apollo 10</t>
   </si>
   <si>
-    <t>Data From Apollo 12 Mission Report</t>
-  </si>
-  <si>
-    <t>CSM at SEP</t>
-  </si>
-  <si>
-    <t>LM at SEP</t>
-  </si>
-  <si>
     <t>Data From Apollo 13 Mission Report &amp; SCOT</t>
   </si>
   <si>
-    <t>CM at SEP</t>
-  </si>
-  <si>
     <t>SLA Ring</t>
   </si>
   <si>
@@ -257,6 +243,12 @@
   </si>
   <si>
     <t>LMRCS</t>
+  </si>
+  <si>
+    <t>Data From Apollo 7 SCOT &amp; Apollo 7 Mission Report</t>
+  </si>
+  <si>
+    <t>Data From Apollo 12 SCOT &amp; Apollo 12 Mission Report</t>
   </si>
 </sst>
 </file>
@@ -378,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -389,7 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,7 +698,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +746,7 @@
         <v>5657.7483494840008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
@@ -769,7 +760,7 @@
         <v>18434.499999999996</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -784,7 +775,7 @@
         <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <f>C38</f>
@@ -798,7 +789,7 @@
         <v>5229.2</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -813,7 +804,7 @@
         <v>20.230219702000003</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <f>C25</f>
@@ -827,7 +818,7 @@
         <v>4661</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -842,7 +833,7 @@
         <v>35.289486386</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="7">
         <f>C30</f>
@@ -856,7 +847,7 @@
         <v>4630.6000000000013</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -871,7 +862,7 @@
         <v>35.607001045000004</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
@@ -882,7 +873,7 @@
         <v>32955.300000000003</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -898,7 +889,7 @@
         <v>111.17548988700001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
@@ -910,7 +901,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f>C2</f>
@@ -932,7 +923,7 @@
         <v>4778.3234625279993</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f>C21</f>
@@ -954,7 +945,7 @@
         <v>7078.7625262199999</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7">
         <f>C7</f>
@@ -1024,7 +1015,7 @@
         <v>49.940519936999998</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1039,7 +1030,7 @@
         <v>102.330438672</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1051,7 +1042,7 @@
         <v>102.285079435</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1062,14 +1053,8 @@
         <f t="shared" si="0"/>
         <v>102.23972019800001</v>
       </c>
-      <c r="E18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18">
-        <v>63720.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1080,14 +1065,8 @@
         <f t="shared" si="0"/>
         <v>102.602594094</v>
       </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19">
-        <v>33499.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1099,14 +1078,8 @@
         <f t="shared" si="0"/>
         <v>609.08383443600007</v>
       </c>
-      <c r="E20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20">
-        <v>12367.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1119,7 +1092,7 @@
         <v>18400.428081419999</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1131,7 +1104,7 @@
         <v>10480.523864272</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1143,7 +1116,7 @@
         <v>2114.1940365700002</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1128,7 @@
         <v>3213.0669121320002</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1167,7 +1140,7 @@
         <v>5148.6816326329999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1180,7 +1153,7 @@
         <v>8361.7485447649997</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1166,7 @@
         <v>2100.4048285220006</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1296,12 +1269,12 @@
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -1322,7 +1295,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,14 +1336,14 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12283.5</v>
+        <v>12363</v>
       </c>
       <c r="C2">
         <f>(CONVERT(B2,"lbm","g"))/1000</f>
-        <v>5571.7018768950002</v>
+        <v>5607.76247031</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
@@ -1384,7 +1357,7 @@
         <v>18429.000000000004</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1399,7 +1372,7 @@
         <v>18.415850222</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <f>C38</f>
@@ -1413,7 +1386,7 @@
         <v>5236.0000000000009</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,21 +1401,21 @@
         <v>18.415850222</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <f>C25</f>
-        <v>2163.680964137</v>
+        <v>2107.6169472050001</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>4770.0999999999995</v>
+        <v>4646.5</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1457,21 +1430,21 @@
         <v>28.848474732000003</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="7">
         <f>C30</f>
-        <v>2335.5924723670005</v>
+        <v>2390.8853822699998</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>5149.1000000000004</v>
+        <v>5271</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1486,18 +1459,18 @@
         <v>28.848474732000003</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
-        <v>15233.536872554003</v>
+        <v>15232.765765525002</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>33584.200000000004</v>
+        <v>33582.5</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1513,11 +1486,11 @@
         <v>94.528649908000006</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
-        <v>4638.7530902790004</v>
+        <v>4766.2579054859998</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
@@ -1525,11 +1498,11 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f>C2</f>
-        <v>5571.7018768950002</v>
+        <v>5607.76247031</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>36</v>
@@ -1540,14 +1513,14 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10226.700000000001</v>
+        <v>10507.8</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>4638.7530902790004</v>
+        <v>4766.2579054859998</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f>C21</f>
@@ -1569,7 +1542,7 @@
         <v>7134.1007953600001</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7">
         <f>C7</f>
@@ -1639,7 +1612,7 @@
         <v>49.895160699999998</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1654,7 +1627,7 @@
         <v>102.05828325</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1666,7 +1639,7 @@
         <v>102.05828325</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1677,18 +1650,8 @@
         <f t="shared" si="0"/>
         <v>101.60469088000001</v>
       </c>
-      <c r="E18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18">
-        <v>63535.6</v>
-      </c>
-      <c r="G18">
-        <f>F18-(B21+B2+B7)</f>
-        <v>10226.699999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1699,14 +1662,8 @@
         <f t="shared" si="0"/>
         <v>102.05828325</v>
       </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19">
-        <v>33584.199999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1719,7 +1676,7 @@
         <v>607.81377580000003</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1732,32 +1689,32 @@
         <v>18514.279766290001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23">
         <f>B2+B9</f>
-        <v>22510.2</v>
+        <v>22870.799999999999</v>
       </c>
       <c r="C23">
         <f>(CONVERT(B23,"lbm","g"))/1000</f>
-        <v>10210.454967174001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10374.020375795999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25">
-        <v>4770.1000000000004</v>
+        <v>4646.5</v>
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C38" si="2">(CONVERT(B25,"lbm","g"))/1000</f>
-        <v>2163.680964137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2107.6169472050001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1769,7 +1726,7 @@
         <v>3210.9803872299999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1781,7 +1738,7 @@
         <v>5148.2733994999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1794,19 +1751,19 @@
         <v>8359.2537867300016</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30">
-        <v>5149.1000000000004</v>
+        <v>5271</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>2335.5924723670005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2390.8853822699998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1818,7 +1775,7 @@
         <v>912.62784844000009</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1916,12 +1873,12 @@
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -1942,7 +1899,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +1948,7 @@
         <v>5458.5759398170003</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
@@ -2005,7 +1962,7 @@
         <v>18184.200000000004</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2020,7 +1977,7 @@
         <v>20.320938175999999</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <f>C38</f>
@@ -2034,7 +1991,7 @@
         <v>5238.3999999999996</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2049,7 +2006,7 @@
         <v>20.139501228</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <f>C25</f>
@@ -2063,7 +2020,7 @@
         <v>4689.7999999999993</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2078,7 +2035,7 @@
         <v>35.561641807999997</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="7">
         <f>C30</f>
@@ -2092,7 +2049,7 @@
         <v>5074.0999999999995</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2107,7 +2064,7 @@
         <v>35.516282571000005</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <f>F2+F3+F4+F5</f>
@@ -2118,7 +2075,7 @@
         <v>33186.5</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2134,7 +2091,7 @@
         <v>111.53836378299999</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
@@ -2146,7 +2103,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f>C2</f>
@@ -2169,7 +2126,7 @@
         <v>4222.4913723299996</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f>C21</f>
@@ -2191,7 +2148,7 @@
         <v>7126.8433174400006</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7">
         <f>C7</f>
@@ -2213,7 +2170,7 @@
         <v>11381.08615567</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F11">
         <f>C20</f>
@@ -2258,7 +2215,7 @@
         <v>63732</v>
       </c>
       <c r="J13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2285,7 +2242,7 @@
         <v>49.895160699999998</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2377,7 +2334,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
         <v>36</v>
@@ -2396,7 +2353,7 @@
         <v>2127.2574968259996</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25">
         <v>33714</v>
@@ -2418,7 +2375,7 @@
         <v>3163.7160622760002</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26">
         <f>F25-(F30+B28)</f>
@@ -2467,7 +2424,7 @@
         <v>2301.5730446170001</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30">
         <v>10840</v>
@@ -2489,7 +2446,7 @@
         <v>916.2112281630001</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F31">
         <f>F30-(B38+F32)</f>
@@ -2512,7 +2469,7 @@
         <v>1459.887042845</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32">
         <v>527.5</v>
@@ -2608,12 +2565,12 @@
         <v>1814.3694800000001</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -2633,8 +2590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,7 +2639,7 @@
         <v>5579.1861510000008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
@@ -2704,7 +2661,7 @@
         <v>19.912705043000003</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <f>C38</f>
@@ -2726,7 +2683,7 @@
         <v>20.003423517000002</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <f>C25</f>
@@ -2748,7 +2705,7 @@
         <v>35.516282571000005</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="7">
         <f>C30</f>
@@ -2783,7 +2740,7 @@
         <v>110.903334465</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
@@ -2795,7 +2752,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f>C2</f>
@@ -2818,7 +2775,7 @@
         <v>4897.8904112600003</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f>C21</f>
@@ -2840,7 +2797,7 @@
         <v>7125.4825403300001</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7">
         <f>C7</f>
@@ -2862,7 +2819,7 @@
         <v>11383.807709890001</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F11">
         <f>C20</f>
@@ -2896,7 +2853,7 @@
         <v>49.623005278000001</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2959,7 +2916,7 @@
         <v>102.375797909</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3186,7 +3143,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B41">
         <v>98</v>
@@ -3206,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="A40:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3255,7 +3212,7 @@
         <v>5476.6742753800008</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
@@ -3285,7 +3242,7 @@
         <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <f>C38</f>
@@ -3307,7 +3264,7 @@
         <v>20.048782754000005</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <f>C25</f>
@@ -3329,7 +3286,7 @@
         <v>35.516282571000005</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="7">
         <f>C30</f>
@@ -3350,14 +3307,14 @@
         <f t="shared" si="0"/>
         <v>35.516282571000005</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>71</v>
+      <c r="E6" t="s">
+        <v>66</v>
       </c>
       <c r="F6">
         <f>C37</f>
         <v>287.57756258000001</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3374,7 +3331,7 @@
         <v>111.13013065000001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
@@ -3394,7 +3351,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f>C2</f>
@@ -3416,7 +3373,7 @@
         <v>4170.5096867279999</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f>C21</f>
@@ -3438,7 +3395,7 @@
         <v>6296.7692803400005</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7">
         <f>C7</f>
@@ -3460,7 +3417,7 @@
         <v>10081.54401562</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F11">
         <f>C20</f>
@@ -3494,7 +3451,7 @@
         <v>49.577646041000001</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3821,8 +3778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3870,7 +3827,7 @@
         <v>5620.9166490400003</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
         <f>C28</f>
@@ -3884,12 +3841,15 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
+      <c r="B3">
+        <v>44.2</v>
+      </c>
       <c r="C3">
         <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
-        <v>0</v>
+        <v>20.048782754000005</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <f>C38</f>
@@ -3903,12 +3863,15 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
+      <c r="B4">
+        <v>44.2</v>
+      </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20.048782754000005</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <f>C25</f>
@@ -3922,12 +3885,15 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
+      <c r="B5">
+        <v>78.7</v>
+      </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35.697719519000003</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="7">
         <f>C30</f>
@@ -3941,9 +3907,12 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
+      <c r="B6">
+        <v>78.2</v>
+      </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35.470923333999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3952,14 +3921,14 @@
       </c>
       <c r="B7">
         <f>B3+B4+B5+B6</f>
-        <v>0</v>
+        <v>245.3</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>111.26620836100001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
         <f>C9</f>
@@ -3971,7 +3940,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f>C2</f>
@@ -3993,11 +3962,11 @@
         <v>4842.0985497500005</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f>C21</f>
-        <v>18408.139151709998</v>
+        <v>18522.898021320001</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>36</v>
@@ -4008,18 +3977,18 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>39917</v>
+        <v>15730.9</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>18106.04663329</v>
+        <v>7135.4162132329993</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7">
-        <f>F15</f>
-        <v>111</v>
+        <f>C7</f>
+        <v>111.26620836100001</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>36</v>
@@ -4027,35 +3996,51 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>666</v>
+        <v>25105.1</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11" si="1">(CONVERT(B11,"lbm","g"))/1000</f>
-        <v>302.09251842000003</v>
+        <v>11387.481808087001</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11">
+        <f>C20</f>
+        <v>608.90239748800002</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
+      <c r="B12">
+        <v>110.6</v>
+      </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50.167316121999995</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
+      <c r="B13">
+        <v>110.2</v>
+      </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49.985879174000004</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13">
         <v>55.5</v>
@@ -4068,12 +4053,15 @@
       <c r="A14" t="s">
         <v>28</v>
       </c>
+      <c r="B14">
+        <v>110.5</v>
+      </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50.121956885000003</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14">
         <v>55.5</v>
@@ -4086,12 +4074,15 @@
       <c r="A15" t="s">
         <v>29</v>
       </c>
+      <c r="B15">
+        <v>109.3</v>
+      </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49.577646041000001</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15">
         <f>F13+F14</f>
@@ -4105,39 +4096,51 @@
       <c r="A16" t="s">
         <v>30</v>
       </c>
+      <c r="B16">
+        <v>226.2</v>
+      </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>102.602594094</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
+      <c r="B17">
+        <v>226.9</v>
+      </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>102.92010875300001</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
+      <c r="B18">
+        <v>224.5</v>
+      </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>101.831487065</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
+      <c r="B19">
+        <v>224.2</v>
+      </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>101.69540935400001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -4146,11 +4149,11 @@
       </c>
       <c r="B20">
         <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
-        <v>0</v>
+        <v>1342.3999999999999</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>608.90239748800002</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4159,11 +4162,11 @@
       </c>
       <c r="B21">
         <f>B10+B11</f>
-        <v>40583</v>
+        <v>40836</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>18408.139151709998</v>
+        <v>18522.898021320001</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4360,6 +4363,635 @@
       <c r="C41">
         <f t="shared" ref="C41" si="3">(CONVERT(B41,"lbm","g"))/1000</f>
         <v>9026.488163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E744F3-3DED-4F12-B13B-2AE7444A35D5}">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" customWidth="1"/>
+    <col min="45" max="45" width="20.5703125" customWidth="1"/>
+    <col min="46" max="46" width="17.28515625" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" customWidth="1"/>
+    <col min="54" max="54" width="17.28515625" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>12384-B7</f>
+        <v>12120.1</v>
+      </c>
+      <c r="C2">
+        <f>(CONVERT(B2,"lbm","g"))/1000</f>
+        <v>5497.5848836370005</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2">
+        <f>C28</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2">
+        <f>SUM(F2:F6)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>CONVERT(I2*1000,"g","lbm")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>44.4</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">(CONVERT(B3,"lbm","g"))/1000</f>
+        <v>20.139501228</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <f>C38</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>44.4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>20.139501228</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <f>C25</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>87.6</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>39.734691611999999</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="7">
+        <f>C30</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>87.5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>39.689332374999999</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6">
+        <f>C37</f>
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>B3+B4+B5+B6</f>
+        <v>263.89999999999998</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>119.703026443</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2">
+        <f>C9</f>
+        <v>3288.0910901299999</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7">
+        <f>SUM(F7:F11)</f>
+        <v>14843.946385960999</v>
+      </c>
+      <c r="J7">
+        <f>CONVERT(I7*1000,"g","lbm")</f>
+        <v>32725.299999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <f>C2</f>
+        <v>5497.5848836370005</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>10604-B20</f>
+        <v>7249</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>3288.0910901299999</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <f>C21</f>
+        <v>4416.7649844009993</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>3710.6</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>1683.0998481219999</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="7">
+        <f>C7</f>
+        <v>119.703026443</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>6026.7</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2733.6651362789999</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11">
+        <f>C20</f>
+        <v>1521.8024013499999</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>111.3</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>50.484830780999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>110.6</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>50.167316121999995</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>110.8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>50.258034595999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>110.6</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>50.167316121999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>223.7</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>101.46861316900001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>2237</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1014.68613169</v>
+      </c>
+      <c r="F17">
+        <v>58962</v>
+      </c>
+      <c r="G17">
+        <f>F17-(B7+B20+B21)</f>
+        <v>45605.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>225.9</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>102.46651638300001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>225.1</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>102.103642487</v>
+      </c>
+      <c r="F19">
+        <v>12319</v>
+      </c>
+      <c r="G19">
+        <f>F19-B7</f>
+        <v>12055.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>B12+B13+B14+B15+B16+B17+B18+B19</f>
+        <v>3355</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1521.8024013499999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B10+B11</f>
+        <v>9737.2999999999993</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>4416.7649844009993</v>
+      </c>
+      <c r="F21">
+        <f>G17-G19</f>
+        <v>33550.700000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <f>B2+B9</f>
+        <v>19369.099999999999</v>
+      </c>
+      <c r="C23">
+        <f>(CONVERT(B23,"lbm","g"))/1000</f>
+        <v>8785.675973767</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C41" si="1">(CONVERT(B25,"lbm","g"))/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>22193</v>
+      </c>
+      <c r="G25">
+        <f>F25-B28</f>
+        <v>22193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <f>B26+B27</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>9807</v>
+      </c>
+      <c r="G30">
+        <f>F30-(B38+B37)</f>
+        <v>9807</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <f>B33+B34+B35+B36</f>
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f>B31+B32</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <v>3852</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40" si="2">(CONVERT(B40,"lbm","g"))/1000</f>
+        <v>1747.2378092400002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41">
+        <v>91</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>41.276905669999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct Apollo 14 and 15 SM oxidizer quantities
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD4388-2641-403C-94AB-3018D66FA2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAEE57-47DF-4321-BCEE-624FC3E40220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1155" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="18" r:id="rId1"/>
@@ -500,6 +500,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,7 +510,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3369,7 +3369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9062379C-30BA-4DAA-98E2-ADF7AF1CF4EB}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -3968,8 +3968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066B9CA6-04BF-488A-87FF-0D836758BC46}">
   <dimension ref="A1:AG18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,60 +4010,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="19"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="10"/>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="20"/>
+      <c r="K1" s="21"/>
       <c r="L1" s="10"/>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="19"/>
+      <c r="N1" s="20"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" s="20"/>
+      <c r="Q1" s="21"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="19"/>
+      <c r="T1" s="20"/>
       <c r="U1" s="10"/>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="W1" s="20"/>
+      <c r="W1" s="21"/>
       <c r="X1" s="10"/>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" s="19"/>
+      <c r="Z1" s="20"/>
       <c r="AA1" s="10"/>
-      <c r="AB1" s="20" t="s">
+      <c r="AB1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" s="20"/>
+      <c r="AC1" s="21"/>
       <c r="AD1" s="10"/>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="19"/>
+      <c r="AF1" s="20"/>
       <c r="AG1" s="10"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="W4" s="17">
         <f>'Apollo 14'!F9</f>
-        <v>13901.880392708003</v>
+        <v>18486.701350193998</v>
       </c>
       <c r="X4" s="12"/>
       <c r="Y4" s="14" t="s">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="Z4" s="18">
         <f>'Apollo 15'!F9</f>
-        <v>13893.080700729999</v>
+        <v>18461.028022052</v>
       </c>
       <c r="AA4" s="12"/>
       <c r="AB4" s="13" t="s">
@@ -4869,11 +4869,11 @@
       </c>
       <c r="V13" t="str">
         <f t="shared" si="7"/>
-        <v>SMFUELLOAD 13901.880392708</v>
+        <v>SMFUELLOAD 18486.701350194</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="8"/>
-        <v>SMFUELLOAD 13893.08070073</v>
+        <v>SMFUELLOAD 18461.028022052</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="9"/>
@@ -5752,7 +5752,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="F9">
         <f>C23</f>
-        <v>13893.080700729999</v>
+        <v>18461.028022052</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>36</v>
@@ -6052,7 +6052,7 @@
       </c>
       <c r="F12">
         <f>C23</f>
-        <v>13893.080700729999</v>
+        <v>18461.028022052</v>
       </c>
       <c r="G12" t="s">
         <v>36</v>
@@ -6063,11 +6063,11 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>14965</v>
+        <v>25035.599999999999</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>6788.0098170500005</v>
+        <v>11355.957138371999</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6188,11 +6188,11 @@
       </c>
       <c r="B23">
         <f>B12+B13</f>
-        <v>30629</v>
+        <v>40699.599999999999</v>
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
-        <v>13893.080700729999</v>
+        <v>18461.028022052</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6408,7 +6408,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="F9">
         <f>C23</f>
-        <v>13901.880392708003</v>
+        <v>18486.701350193998</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>36</v>
@@ -6709,11 +6709,11 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>14953.2</v>
+        <v>25061</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>6782.657427084001</v>
+        <v>11367.47838457</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6834,11 +6834,11 @@
       </c>
       <c r="B23">
         <f>B12+B13</f>
-        <v>30648.400000000001</v>
+        <v>40756.199999999997</v>
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
-        <v>13901.880392708003</v>
+        <v>18486.701350193998</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -8777,7 +8777,7 @@
         <f t="shared" si="2"/>
         <v>102.05828325</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="19">
         <v>4222.4913720000004</v>
       </c>
       <c r="F21">

</xml_diff>

<commit_message>
Update Apollo 14 SM empty mass to include post Apollo 13 additions
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAEE57-47DF-4321-BCEE-624FC3E40220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016DC01E-19C9-46EE-A1FD-0B9DA06C5DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="85">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>Data From Apollo XX</t>
+  </si>
+  <si>
+    <t>Post 13 Added Mass</t>
   </si>
 </sst>
 </file>
@@ -3969,7 +3972,7 @@
   <dimension ref="A1:AG18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4128,7 +4131,7 @@
       </c>
       <c r="W2" s="17">
         <f>'Apollo 14'!F7</f>
-        <v>4213.5556026409995</v>
+        <v>4512.9265668409998</v>
       </c>
       <c r="X2" s="12"/>
       <c r="Y2" s="14" t="s">
@@ -4777,7 +4780,7 @@
       </c>
       <c r="V11" t="str">
         <f>V2&amp;" "&amp;W2</f>
-        <v>SMMASS 4213.555602641</v>
+        <v>SMMASS 4512.926566841</v>
       </c>
       <c r="Y11" t="str">
         <f>Y2&amp;" "&amp;Z2</f>
@@ -6408,7 +6411,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6606,7 +6609,7 @@
       </c>
       <c r="F7" s="2">
         <f>C11</f>
-        <v>4213.5556026409995</v>
+        <v>4512.9265668409998</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
@@ -6674,12 +6677,12 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <f>B10-B22+B43</f>
-        <v>9289.2999999999993</v>
+        <f>B10-B22+B43+F19</f>
+        <v>9949.2999999999993</v>
       </c>
       <c r="C11">
         <f t="shared" si="3"/>
-        <v>4213.5556026409995</v>
+        <v>4512.9265668409998</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
@@ -6755,7 +6758,7 @@
         <v>50.076597648000003</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -6767,7 +6770,7 @@
         <v>49.759082988999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -6779,7 +6782,7 @@
         <v>102.19436096100002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -6790,8 +6793,18 @@
         <f t="shared" si="2"/>
         <v>102.149001724</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19">
+        <v>660</v>
+      </c>
+      <c r="G19">
+        <f>(CONVERT(F19,"lbm","g"))/1000</f>
+        <v>299.3709642</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -6803,7 +6816,7 @@
         <v>102.73867180500001</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -6815,7 +6828,7 @@
         <v>101.37789469500001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -6828,7 +6841,7 @@
         <v>608.08593122199989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -6841,7 +6854,7 @@
         <v>18486.701350193998</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -6854,7 +6867,7 @@
         <v>10381.550009138002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -6866,7 +6879,7 @@
         <v>2166.3117998830003</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -6878,7 +6891,7 @@
         <v>3208.1681145360003</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -6890,7 +6903,7 @@
         <v>5145.7332822280005</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -6903,7 +6916,7 @@
         <v>8353.9013967640003</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -7053,8 +7066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67D65E4-4F47-4D15-8C66-BD009E2D808A}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7699,7 +7712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DAF9E-BC71-4638-95FD-6BF28D732C5B}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Apollo 5 to mass spreadsheets
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016DC01E-19C9-46EE-A1FD-0B9DA06C5DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A68A78E-8119-4465-ABB7-6F9BC99E0815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="88">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -305,6 +305,15 @@
   <si>
     <t>Post 13 Added Mass</t>
   </si>
+  <si>
+    <t>Nose Cap</t>
+  </si>
+  <si>
+    <t>Apollo 5</t>
+  </si>
+  <si>
+    <t>Data From Apollo 5 SCOT &amp; Apollo 5 Mission Report</t>
+  </si>
 </sst>
 </file>
 
@@ -504,13 +513,13 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2121,7 +2130,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72429DAA-B9F6-4DDA-BFC1-E3E1D001C964}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,18 +2832,18 @@
       </c>
       <c r="F2" s="2">
         <f>C30</f>
-        <v>0</v>
+        <v>8121.57138485</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I2">
         <f>SUM(F2:F6)</f>
-        <v>0</v>
+        <v>14305.668320482</v>
       </c>
       <c r="J2">
         <f>CONVERT(I2*1000,"g","lbm")</f>
-        <v>0</v>
+        <v>31538.600000000002</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2854,7 +2863,7 @@
       </c>
       <c r="F3">
         <f>C40</f>
-        <v>0</v>
+        <v>2341.89740631</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>36</v>
@@ -2873,7 +2882,7 @@
       </c>
       <c r="F4">
         <f>C27</f>
-        <v>0</v>
+        <v>1478.7111262000001</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>36</v>
@@ -2892,7 +2901,7 @@
       </c>
       <c r="F5" s="7">
         <f>C32</f>
-        <v>0</v>
+        <v>2086.0713096300001</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>36</v>
@@ -2911,7 +2920,7 @@
       </c>
       <c r="F6">
         <f>C39</f>
-        <v>0</v>
+        <v>277.41709349199999</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -3002,10 +3011,6 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <f>B10-B22+B43</f>
-        <v>0</v>
-      </c>
       <c r="C11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3039,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3175,7 +3180,7 @@
       </c>
       <c r="G25">
         <f>F25-B30</f>
-        <v>22193</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3183,11 +3188,11 @@
         <v>3</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>3260</v>
       </c>
       <c r="C27">
         <f t="shared" ref="C27:C43" si="1">(CONVERT(B27,"lbm","g"))/1000</f>
-        <v>0</v>
+        <v>1478.7111262000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3195,11 +3200,11 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>6957</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3155.6421180900002</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3207,11 +3212,11 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>10948</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4965.9292667600002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3220,18 +3225,18 @@
       </c>
       <c r="B30">
         <f>B28+B29</f>
-        <v>0</v>
+        <v>17905</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8121.57138485</v>
       </c>
       <c r="F30">
         <v>9807</v>
       </c>
       <c r="G30">
         <f>F30-(B40+B39)</f>
-        <v>9807</v>
+        <v>4032.3999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3239,127 +3244,137 @@
         <v>12</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>4599</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2086.0713096300001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1993</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>904.00959341000009</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>3170</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1437.8878129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46.266421740000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>102.8</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46.629295636000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>203.4</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92.260688058</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>203.4</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92.260688058</v>
+      </c>
+      <c r="F38">
+        <f>B27+B30+B32+B39+B40</f>
+        <v>31538.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
       <c r="B39">
         <f>B35+B36+B37+B38</f>
-        <v>0</v>
+        <v>611.6</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>277.41709349199999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="B40">
         <f>B33+B34</f>
-        <v>0</v>
+        <v>5163</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2341.89740631</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
+      <c r="B42">
+        <v>3950</v>
+      </c>
       <c r="C42">
         <f t="shared" ref="C42" si="2">(CONVERT(B42,"lbm","g"))/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1791.6898615</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>85</v>
+      </c>
+      <c r="B43">
+        <v>1067</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>483.98305879000003</v>
       </c>
     </row>
   </sheetData>
@@ -3969,10 +3984,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066B9CA6-04BF-488A-87FF-0D836758BC46}">
-  <dimension ref="A1:AG18"/>
+  <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,7 +3996,7 @@
     <col min="2" max="2" width="10.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="16" bestFit="1" customWidth="1"/>
@@ -4010,1094 +4025,1163 @@
     <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="4.5703125" customWidth="1"/>
+    <col min="34" max="34" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="22"/>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="21"/>
       <c r="C1" s="10"/>
       <c r="D1" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="21"/>
       <c r="F1" s="10"/>
       <c r="G1" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="10"/>
-      <c r="J1" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="21"/>
+      <c r="J1" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="22"/>
       <c r="L1" s="10"/>
       <c r="M1" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N1" s="20"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="21"/>
+      <c r="P1" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="22"/>
       <c r="R1" s="10"/>
       <c r="S1" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T1" s="20"/>
       <c r="U1" s="10"/>
-      <c r="V1" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="W1" s="21"/>
+      <c r="V1" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" s="22"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z1" s="20"/>
       <c r="AA1" s="10"/>
-      <c r="AB1" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC1" s="21"/>
+      <c r="AB1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC1" s="22"/>
       <c r="AD1" s="10"/>
       <c r="AE1" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AF1" s="20"/>
       <c r="AG1" s="10"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="10"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="15">
+        <f>'Apollo 5'!F2</f>
+        <v>8121.57138485</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="15">
+      <c r="E2" s="15">
         <f>'Apollo 7'!F7</f>
         <v>4242.5855143209992</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="17">
+      <c r="H2" s="17">
         <f>'Apollo 8'!F7</f>
         <v>4277.6482045220009</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="14" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="18">
+      <c r="K2" s="18">
         <f>'Apollo 9'!F7</f>
         <v>4270.7536004980002</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13" t="s">
+      <c r="L2" s="12"/>
+      <c r="M2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="17">
+      <c r="N2" s="17">
         <f>'Apollo 10'!F7</f>
         <v>4289.668402327</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="14" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="18">
+      <c r="Q2" s="18">
         <f>'Apollo 11'!F7</f>
         <v>4266.9434245900002</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13" t="s">
+      <c r="R2" s="12"/>
+      <c r="S2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="T2" s="17">
         <f>'Apollo 12'!F7</f>
         <v>4202.8961819460001</v>
       </c>
-      <c r="R2" s="12"/>
-      <c r="S2" s="14" t="s">
+      <c r="U2" s="12"/>
+      <c r="V2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="18">
+      <c r="W2" s="18">
         <f>'Apollo 13'!F7</f>
         <v>4213.6916803519998</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="13" t="s">
+      <c r="X2" s="12"/>
+      <c r="Y2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="17">
+      <c r="Z2" s="17">
         <f>'Apollo 14'!F7</f>
         <v>4512.9265668409998</v>
       </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="14" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" s="18">
+      <c r="AC2" s="18">
         <f>'Apollo 15'!F7</f>
         <v>5550.5191132159998</v>
       </c>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="13" t="s">
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="17">
+      <c r="AF2" s="17">
         <f>'Apollo 16'!F7</f>
         <v>5540.2679256540005</v>
       </c>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="14" t="s">
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AF2" s="18">
+      <c r="AI2" s="18">
         <f>'Apollo 17'!F7</f>
         <v>5536.0948758500008</v>
       </c>
-      <c r="AG2" s="12"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="12"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="15">
+        <f>'Apollo 5'!F3</f>
+        <v>2341.89740631</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="15">
+      <c r="E3" s="15">
         <f>'Apollo 7'!F8</f>
         <v>5497.5848836370005</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="17">
+      <c r="H3" s="17">
         <f>'Apollo 8'!F8</f>
         <v>5509.6504406790009</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="14" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="18">
+      <c r="K3" s="18">
         <f>'Apollo 9'!F8</f>
         <v>5476.6742753800008</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13" t="s">
+      <c r="L3" s="12"/>
+      <c r="M3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="17">
+      <c r="N3" s="17">
         <f>'Apollo 10'!F8</f>
         <v>5468.2828165350002</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="14" t="s">
+      <c r="O3" s="12"/>
+      <c r="P3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="18">
+      <c r="Q3" s="18">
         <f>'Apollo 11'!F8</f>
         <v>5458.5759398170003</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="13" t="s">
+      <c r="R3" s="12"/>
+      <c r="S3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="T3" s="17">
         <f>'Apollo 12'!F8</f>
         <v>5513.2338204019998</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="14" t="s">
+      <c r="U3" s="12"/>
+      <c r="V3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="18">
+      <c r="W3" s="18">
         <f>'Apollo 13'!F8</f>
         <v>5546.5728595970004</v>
       </c>
-      <c r="U3" s="12"/>
-      <c r="V3" s="13" t="s">
+      <c r="X3" s="12"/>
+      <c r="Y3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="17">
+      <c r="Z3" s="17">
         <f>'Apollo 14'!F8</f>
         <v>5604.3605275350001</v>
       </c>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="14" t="s">
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="18">
+      <c r="AC3" s="18">
         <f>'Apollo 15'!F8</f>
         <v>5723.6553208450005</v>
       </c>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="13" t="s">
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="17">
+      <c r="AF3" s="17">
         <f>'Apollo 16'!F8</f>
         <v>5678.7496762150004</v>
       </c>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="14" t="s">
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AF3" s="18">
+      <c r="AI3" s="18">
         <f>'Apollo 17'!F8</f>
         <v>5734.7683339100004</v>
       </c>
-      <c r="AG3" s="12"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ3" s="12"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="15">
+        <f>'Apollo 5'!F4</f>
+        <v>1478.7111262000001</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="15">
+      <c r="E4" s="15">
         <f>'Apollo 7'!F9</f>
         <v>4416.7649844009993</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="17">
+      <c r="H4" s="17">
         <f>'Apollo 8'!F9</f>
         <v>18522.898021320001</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="14" t="s">
+      <c r="I4" s="12"/>
+      <c r="J4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="18">
+      <c r="K4" s="18">
         <f>'Apollo 9'!F9</f>
         <v>16378.313295960001</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13" t="s">
+      <c r="L4" s="12"/>
+      <c r="M4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="17">
+      <c r="N4" s="17">
         <f>'Apollo 10'!F9</f>
         <v>18509.290250220001</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="14" t="s">
+      <c r="O4" s="12"/>
+      <c r="P4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="18">
+      <c r="Q4" s="18">
         <f>'Apollo 11'!F9</f>
         <v>18507.929473110002</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13" t="s">
+      <c r="R4" s="12"/>
+      <c r="S4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="T4" s="17">
         <f>'Apollo 12'!F9</f>
         <v>18514.279766290001</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="14" t="s">
+      <c r="U4" s="12"/>
+      <c r="V4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="18">
+      <c r="W4" s="18">
         <f>'Apollo 13'!F9</f>
         <v>18400.428081419999</v>
       </c>
-      <c r="U4" s="12"/>
-      <c r="V4" s="13" t="s">
+      <c r="X4" s="12"/>
+      <c r="Y4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="17">
+      <c r="Z4" s="17">
         <f>'Apollo 14'!F9</f>
         <v>18486.701350193998</v>
       </c>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="14" t="s">
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="Z4" s="18">
+      <c r="AC4" s="18">
         <f>'Apollo 15'!F9</f>
         <v>18461.028022052</v>
       </c>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="13" t="s">
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AC4" s="17">
+      <c r="AF4" s="17">
         <f>'Apollo 16'!F9</f>
         <v>18482.301504204999</v>
       </c>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="14" t="s">
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AF4" s="18">
+      <c r="AI4" s="18">
         <f>'Apollo 17'!F9</f>
         <v>18480.26033854</v>
       </c>
-      <c r="AG4" s="12"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="12"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="15">
+        <f>'Apollo 5'!F5</f>
+        <v>2086.0713096300001</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="15">
+      <c r="E5" s="15">
         <f>'Apollo 7'!F10</f>
         <v>119.703026443</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="17">
+      <c r="H5" s="17">
         <f>'Apollo 8'!F10</f>
         <v>111.26620836100001</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="14" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="18">
+      <c r="K5" s="18">
         <f>'Apollo 9'!F10</f>
         <v>111.13013065000001</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13" t="s">
+      <c r="L5" s="12"/>
+      <c r="M5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="17">
+      <c r="N5" s="17">
         <f>'Apollo 10'!F10</f>
         <v>110.903334465</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="14" t="s">
+      <c r="O5" s="12"/>
+      <c r="P5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="N5" s="18">
+      <c r="Q5" s="18">
         <f>'Apollo 11'!F10</f>
         <v>111.53836378299999</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13" t="s">
+      <c r="R5" s="12"/>
+      <c r="S5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="T5" s="17">
         <f>'Apollo 12'!F10</f>
         <v>94.528649908000006</v>
       </c>
-      <c r="R5" s="12"/>
-      <c r="S5" s="14" t="s">
+      <c r="U5" s="12"/>
+      <c r="V5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="18">
+      <c r="W5" s="18">
         <f>'Apollo 13'!F10</f>
         <v>111.17548988700001</v>
       </c>
-      <c r="U5" s="12"/>
-      <c r="V5" s="13" t="s">
+      <c r="X5" s="12"/>
+      <c r="Y5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="W5" s="17">
+      <c r="Z5" s="17">
         <f>'Apollo 14'!F10</f>
         <v>111.356926835</v>
       </c>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="14" t="s">
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Z5" s="18">
+      <c r="AC5" s="18">
         <f>'Apollo 15'!F10</f>
         <v>110.903334465</v>
       </c>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="13" t="s">
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AC5" s="17">
+      <c r="AF5" s="17">
         <f>'Apollo 16'!F10</f>
         <v>105.86845915799999</v>
       </c>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="14" t="s">
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AF5" s="18">
+      <c r="AI5" s="18">
         <f>'Apollo 17'!F10</f>
         <v>105.68702221000001</v>
       </c>
-      <c r="AG5" s="12"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="12"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="15"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="18">
+      <c r="K6" s="18">
         <f>'Apollo 9'!F2</f>
         <v>8182.8063548</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13" t="s">
+      <c r="L6" s="12"/>
+      <c r="M6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="17">
+      <c r="N6" s="17">
         <f>'Apollo 10'!F2</f>
         <v>8263.8633113190008</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="14" t="s">
+      <c r="O6" s="12"/>
+      <c r="P6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="N6" s="18">
+      <c r="Q6" s="18">
         <f>'Apollo 11'!F2</f>
         <v>8248.2143745540016</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13" t="s">
+      <c r="R6" s="12"/>
+      <c r="S6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="T6" s="17">
         <f>'Apollo 12'!F2</f>
         <v>8359.2537867300016</v>
       </c>
-      <c r="R6" s="12"/>
-      <c r="S6" s="14" t="s">
+      <c r="U6" s="12"/>
+      <c r="V6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="18">
+      <c r="W6" s="18">
         <f>'Apollo 13'!F2</f>
         <v>8361.7485447649997</v>
       </c>
-      <c r="U6" s="12"/>
-      <c r="V6" s="13" t="s">
+      <c r="X6" s="12"/>
+      <c r="Y6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="W6" s="17">
+      <c r="Z6" s="17">
         <f>'Apollo 14'!F2</f>
         <v>8353.9013967640003</v>
       </c>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="14" t="s">
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z6" s="18">
+      <c r="AC6" s="18">
         <f>'Apollo 15'!F2</f>
         <v>8872.9471457550007</v>
       </c>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="13" t="s">
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AC6" s="17">
+      <c r="AF6" s="17">
         <f>'Apollo 16'!F2</f>
         <v>8871.9492425410008</v>
       </c>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="14" t="s">
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF6" s="18">
+      <c r="AI6" s="18">
         <f>'Apollo 17'!F2</f>
         <v>8874.171845154</v>
       </c>
-      <c r="AG6" s="12"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="12"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="15"/>
       <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="18">
+      <c r="K7" s="18">
         <f>'Apollo 9'!F3</f>
         <v>1882.4083355</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13" t="s">
+      <c r="L7" s="12"/>
+      <c r="M7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="17">
+      <c r="N7" s="17">
         <f>'Apollo 10'!F3</f>
         <v>1193.40152547</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="14" t="s">
+      <c r="O7" s="12"/>
+      <c r="P7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="18">
+      <c r="Q7" s="18">
         <f>'Apollo 11'!F3</f>
         <v>2376.0982710079998</v>
       </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13" t="s">
+      <c r="R7" s="12"/>
+      <c r="S7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="T7" s="17">
         <f>'Apollo 12'!F3</f>
         <v>2375.0096493200003</v>
       </c>
-      <c r="R7" s="12"/>
-      <c r="S7" s="14" t="s">
+      <c r="U7" s="12"/>
+      <c r="V7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="18">
+      <c r="W7" s="18">
         <f>'Apollo 13'!F3</f>
         <v>2371.9252212040001</v>
       </c>
-      <c r="U7" s="12"/>
-      <c r="V7" s="13" t="s">
+      <c r="X7" s="12"/>
+      <c r="Y7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="W7" s="17">
+      <c r="Z7" s="17">
         <f>'Apollo 14'!F3</f>
         <v>2370.110851724</v>
       </c>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="14" t="s">
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="Z7" s="18">
+      <c r="AC7" s="18">
         <f>'Apollo 15'!F3</f>
         <v>2375.4632416899999</v>
       </c>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="13" t="s">
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AC7" s="17">
+      <c r="AF7" s="17">
         <f>'Apollo 16'!F3</f>
         <v>2377.9579997249998</v>
       </c>
-      <c r="AD7" s="12"/>
-      <c r="AE7" s="14" t="s">
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AF7" s="18">
+      <c r="AI7" s="18">
         <f>'Apollo 17'!F3</f>
         <v>2386.6669732290002</v>
       </c>
-      <c r="AG7" s="12"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="12"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="15"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="17"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="18">
+      <c r="K8" s="18">
         <f>'Apollo 9'!F4</f>
         <v>1883.7691126100001</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13" t="s">
+      <c r="L8" s="12"/>
+      <c r="M8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="17">
+      <c r="N8" s="17">
         <f>'Apollo 10'!F4</f>
         <v>2133.2449161100003</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="14" t="s">
+      <c r="O8" s="12"/>
+      <c r="P8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="18">
+      <c r="Q8" s="18">
         <f>'Apollo 11'!F4</f>
         <v>2127.2574968259996</v>
       </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13" t="s">
+      <c r="R8" s="12"/>
+      <c r="S8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="T8" s="17">
         <f>'Apollo 12'!F4</f>
         <v>2107.6169472050001</v>
       </c>
-      <c r="R8" s="12"/>
-      <c r="S8" s="14" t="s">
+      <c r="U8" s="12"/>
+      <c r="V8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T8" s="18">
+      <c r="W8" s="18">
         <f>'Apollo 13'!F4</f>
         <v>2109.2045204999999</v>
       </c>
-      <c r="U8" s="12"/>
-      <c r="V8" s="13" t="s">
+      <c r="X8" s="12"/>
+      <c r="Y8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="W8" s="17">
+      <c r="Z8" s="17">
         <f>'Apollo 14'!F4</f>
         <v>2166.3117998830003</v>
       </c>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="14" t="s">
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="Z8" s="18">
+      <c r="AC8" s="18">
         <f>'Apollo 15'!F4</f>
         <v>2802.7472542300002</v>
       </c>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="13" t="s">
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="17">
+      <c r="AF8" s="17">
         <f>'Apollo 16'!F4</f>
         <v>2793.9929214889999</v>
       </c>
-      <c r="AD8" s="12"/>
-      <c r="AE8" s="14" t="s">
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AF8" s="18">
+      <c r="AI8" s="18">
         <f>'Apollo 17'!F4</f>
         <v>2791.7249596390002</v>
       </c>
-      <c r="AG8" s="12"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="12"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="15"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="17"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="18">
+      <c r="K9" s="18">
         <f>'Apollo 9'!F5</f>
         <v>2278.3944745100002</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13" t="s">
+      <c r="L9" s="12"/>
+      <c r="M9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="17">
+      <c r="N9" s="17">
         <f>'Apollo 10'!F5</f>
         <v>2446.22365141</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="14" t="s">
+      <c r="O9" s="12"/>
+      <c r="P9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="18">
+      <c r="Q9" s="18">
         <f>'Apollo 11'!F5</f>
         <v>2301.5730446170001</v>
       </c>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13" t="s">
+      <c r="R9" s="12"/>
+      <c r="S9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="T9" s="17">
         <f>'Apollo 12'!F5</f>
         <v>2103.3078196900001</v>
       </c>
-      <c r="R9" s="12"/>
-      <c r="S9" s="14" t="s">
+      <c r="U9" s="12"/>
+      <c r="V9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="T9" s="18">
+      <c r="W9" s="18">
         <f>'Apollo 13'!F5</f>
         <v>2090.425796382</v>
       </c>
-      <c r="U9" s="12"/>
-      <c r="V9" s="13" t="s">
+      <c r="X9" s="12"/>
+      <c r="Y9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="W9" s="17">
+      <c r="Z9" s="17">
         <f>'Apollo 14'!F5</f>
         <v>2103.3078196900001</v>
       </c>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="14" t="s">
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="Z9" s="18">
+      <c r="AC9" s="18">
         <f>'Apollo 15'!F5</f>
         <v>2132.4738090810001</v>
       </c>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="13" t="s">
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AC9" s="17">
+      <c r="AF9" s="17">
         <f>'Apollo 16'!F5</f>
         <v>2141.727093429</v>
       </c>
-      <c r="AD9" s="12"/>
-      <c r="AE9" s="14" t="s">
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AF9" s="18">
+      <c r="AI9" s="18">
         <f>'Apollo 17'!F5</f>
         <v>2144.6754438339999</v>
       </c>
-      <c r="AG9" s="12"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ9" s="12"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>A2&amp;" "&amp;B2</f>
-        <v>SMMASS 4242.585514321</v>
+        <v>LMDSCFUEL 8121.57138485</v>
       </c>
       <c r="D11" t="str">
         <f>D2&amp;" "&amp;E2</f>
-        <v>SMMASS 4277.648204522</v>
+        <v>SMMASS 4242.585514321</v>
       </c>
       <c r="G11" t="str">
         <f>G2&amp;" "&amp;H2</f>
-        <v>SMMASS 4270.753600498</v>
+        <v>SMMASS 4277.648204522</v>
       </c>
       <c r="J11" t="str">
         <f>J2&amp;" "&amp;K2</f>
-        <v>SMMASS 4289.668402327</v>
+        <v>SMMASS 4270.753600498</v>
       </c>
       <c r="M11" t="str">
         <f>M2&amp;" "&amp;N2</f>
-        <v>SMMASS 4266.94342459</v>
+        <v>SMMASS 4289.668402327</v>
       </c>
       <c r="P11" t="str">
         <f>P2&amp;" "&amp;Q2</f>
-        <v>SMMASS 4202.896181946</v>
+        <v>SMMASS 4266.94342459</v>
       </c>
       <c r="S11" t="str">
         <f>S2&amp;" "&amp;T2</f>
-        <v>SMMASS 4213.691680352</v>
+        <v>SMMASS 4202.896181946</v>
       </c>
       <c r="V11" t="str">
         <f>V2&amp;" "&amp;W2</f>
-        <v>SMMASS 4512.926566841</v>
+        <v>SMMASS 4213.691680352</v>
       </c>
       <c r="Y11" t="str">
         <f>Y2&amp;" "&amp;Z2</f>
-        <v>SMMASS 5550.519113216</v>
+        <v>SMMASS 4512.926566841</v>
       </c>
       <c r="AB11" t="str">
         <f>AB2&amp;" "&amp;AC2</f>
-        <v>SMMASS 5540.267925654</v>
+        <v>SMMASS 5550.519113216</v>
       </c>
       <c r="AE11" t="str">
         <f>AE2&amp;" "&amp;AF2</f>
+        <v>SMMASS 5540.267925654</v>
+      </c>
+      <c r="AH11" t="str">
+        <f>AH2&amp;" "&amp;AI2</f>
         <v>SMMASS 5536.09487585</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" ref="A12:A14" si="0">A3&amp;" "&amp;B3</f>
-        <v>CMMASS 5497.584883637</v>
+        <v>LMASCFUEL 2341.89740631</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ref="D12:D14" si="1">D3&amp;" "&amp;E3</f>
+        <v>CMMASS 5497.584883637</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ref="G12:G14" si="2">G3&amp;" "&amp;H3</f>
         <v>CMMASS 5509.650440679</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" ref="G12:G18" si="2">G3&amp;" "&amp;H3</f>
-        <v>CMMASS 5476.67427538</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" ref="J12:J18" si="3">J3&amp;" "&amp;K3</f>
-        <v>CMMASS 5468.282816535</v>
+        <v>CMMASS 5476.67427538</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ref="M12:M18" si="4">M3&amp;" "&amp;N3</f>
-        <v>CMMASS 5458.575939817</v>
+        <v>CMMASS 5468.282816535</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" ref="P12:P18" si="5">P3&amp;" "&amp;Q3</f>
-        <v>CMMASS 5513.233820402</v>
+        <v>CMMASS 5458.575939817</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" ref="S12:S18" si="6">S3&amp;" "&amp;T3</f>
-        <v>CMMASS 5546.572859597</v>
+        <v>CMMASS 5513.233820402</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" ref="V12:V18" si="7">V3&amp;" "&amp;W3</f>
-        <v>CMMASS 5604.360527535</v>
+        <v>CMMASS 5546.572859597</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" ref="Y12:Y18" si="8">Y3&amp;" "&amp;Z3</f>
-        <v>CMMASS 5723.655320845</v>
+        <v>CMMASS 5604.360527535</v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" ref="AB12:AB18" si="9">AB3&amp;" "&amp;AC3</f>
+        <v>CMMASS 5723.655320845</v>
+      </c>
+      <c r="AE12" t="str">
+        <f t="shared" ref="AE12:AE18" si="10">AE3&amp;" "&amp;AF3</f>
         <v>CMMASS 5678.749676215</v>
       </c>
-      <c r="AE12" t="str">
-        <f t="shared" ref="AE12:AE17" si="10">AE3&amp;" "&amp;AF3</f>
+      <c r="AH12" t="str">
+        <f t="shared" ref="AH12:AH17" si="11">AH3&amp;" "&amp;AI3</f>
         <v>CMMASS 5734.76833391</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>SMFUELLOAD 4416.764984401</v>
+        <v>LMDSCEMPTY 1478.7111262</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
+        <v>SMFUELLOAD 4416.764984401</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
         <v>SMFUELLOAD 18522.89802132</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="2"/>
-        <v>SMFUELLOAD 16378.31329596</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="3"/>
-        <v>SMFUELLOAD 18509.29025022</v>
+        <v>SMFUELLOAD 16378.31329596</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="4"/>
-        <v>SMFUELLOAD 18507.92947311</v>
+        <v>SMFUELLOAD 18509.29025022</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="5"/>
-        <v>SMFUELLOAD 18514.27976629</v>
+        <v>SMFUELLOAD 18507.92947311</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="6"/>
-        <v>SMFUELLOAD 18400.42808142</v>
+        <v>SMFUELLOAD 18514.27976629</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="7"/>
-        <v>SMFUELLOAD 18486.701350194</v>
+        <v>SMFUELLOAD 18400.42808142</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="8"/>
-        <v>SMFUELLOAD 18461.028022052</v>
+        <v>SMFUELLOAD 18486.701350194</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="9"/>
-        <v>SMFUELLOAD 18482.301504205</v>
+        <v>SMFUELLOAD 18461.028022052</v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="10"/>
+        <v>SMFUELLOAD 18482.301504205</v>
+      </c>
+      <c r="AH13" t="str">
+        <f t="shared" si="11"/>
         <v>SMFUELLOAD 18480.26033854</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>CMFUELLOAD 119.703026443</v>
+        <v>LMASCEMPTY 2086.07130963</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
+        <v>CMFUELLOAD 119.703026443</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
         <v>CMFUELLOAD 111.266208361</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="2"/>
-        <v>CMFUELLOAD 111.13013065</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>CMFUELLOAD 110.903334465</v>
+        <v>CMFUELLOAD 111.13013065</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="4"/>
-        <v>CMFUELLOAD 111.538363783</v>
+        <v>CMFUELLOAD 110.903334465</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="5"/>
-        <v>CMFUELLOAD 94.528649908</v>
+        <v>CMFUELLOAD 111.538363783</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="6"/>
-        <v>CMFUELLOAD 111.175489887</v>
+        <v>CMFUELLOAD 94.528649908</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="7"/>
-        <v>CMFUELLOAD 111.356926835</v>
+        <v>CMFUELLOAD 111.175489887</v>
       </c>
       <c r="Y14" t="str">
         <f t="shared" si="8"/>
-        <v>CMFUELLOAD 110.903334465</v>
+        <v>CMFUELLOAD 111.356926835</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="9"/>
-        <v>CMFUELLOAD 105.868459158</v>
+        <v>CMFUELLOAD 110.903334465</v>
       </c>
       <c r="AE14" t="str">
         <f t="shared" si="10"/>
+        <v>CMFUELLOAD 105.868459158</v>
+      </c>
+      <c r="AH14" t="str">
+        <f t="shared" si="11"/>
         <v>CMFUELLOAD 105.68702221</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="G15" t="str">
-        <f t="shared" si="2"/>
-        <v>LMDSCFUEL 8182.8063548</v>
-      </c>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>LMDSCFUEL 8263.863311319</v>
+        <v>LMDSCFUEL 8182.8063548</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="4"/>
-        <v>LMDSCFUEL 8248.214374554</v>
+        <v>LMDSCFUEL 8263.863311319</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="5"/>
-        <v>LMDSCFUEL 8359.25378673</v>
+        <v>LMDSCFUEL 8248.214374554</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="6"/>
-        <v>LMDSCFUEL 8361.748544765</v>
+        <v>LMDSCFUEL 8359.25378673</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="7"/>
-        <v>LMDSCFUEL 8353.901396764</v>
+        <v>LMDSCFUEL 8361.748544765</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="8"/>
-        <v>LMDSCFUEL 8872.947145755</v>
+        <v>LMDSCFUEL 8353.901396764</v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="9"/>
-        <v>LMDSCFUEL 8871.949242541</v>
+        <v>LMDSCFUEL 8872.947145755</v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="10"/>
+        <v>LMDSCFUEL 8871.949242541</v>
+      </c>
+      <c r="AH15" t="str">
+        <f t="shared" si="11"/>
         <v>LMDSCFUEL 8874.171845154</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="G16" t="str">
-        <f t="shared" si="2"/>
-        <v>LMASCFUEL 1882.4083355</v>
-      </c>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>LMASCFUEL 1193.40152547</v>
+        <v>LMASCFUEL 1882.4083355</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="4"/>
-        <v>LMASCFUEL 2376.098271008</v>
+        <v>LMASCFUEL 1193.40152547</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="5"/>
-        <v>LMASCFUEL 2375.00964932</v>
+        <v>LMASCFUEL 2376.098271008</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="6"/>
-        <v>LMASCFUEL 2371.925221204</v>
+        <v>LMASCFUEL 2375.00964932</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="7"/>
-        <v>LMASCFUEL 2370.110851724</v>
+        <v>LMASCFUEL 2371.925221204</v>
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="8"/>
-        <v>LMASCFUEL 2375.46324169</v>
+        <v>LMASCFUEL 2370.110851724</v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="9"/>
-        <v>LMASCFUEL 2377.957999725</v>
+        <v>LMASCFUEL 2375.46324169</v>
       </c>
       <c r="AE16" t="str">
         <f t="shared" si="10"/>
+        <v>LMASCFUEL 2377.957999725</v>
+      </c>
+      <c r="AH16" t="str">
+        <f t="shared" si="11"/>
         <v>LMASCFUEL 2386.666973229</v>
       </c>
     </row>
-    <row r="17" spans="7:31" x14ac:dyDescent="0.25">
-      <c r="G17" t="str">
-        <f t="shared" si="2"/>
-        <v>LMDSCEMPTY 1883.76911261</v>
-      </c>
+    <row r="17" spans="10:34" x14ac:dyDescent="0.25">
       <c r="J17" t="str">
         <f t="shared" si="3"/>
-        <v>LMDSCEMPTY 2133.24491611</v>
+        <v>LMDSCEMPTY 1883.76911261</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="4"/>
-        <v>LMDSCEMPTY 2127.257496826</v>
+        <v>LMDSCEMPTY 2133.24491611</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="5"/>
-        <v>LMDSCEMPTY 2107.616947205</v>
+        <v>LMDSCEMPTY 2127.257496826</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="6"/>
-        <v>LMDSCEMPTY 2109.2045205</v>
+        <v>LMDSCEMPTY 2107.616947205</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="7"/>
-        <v>LMDSCEMPTY 2166.311799883</v>
+        <v>LMDSCEMPTY 2109.2045205</v>
       </c>
       <c r="Y17" t="str">
         <f t="shared" si="8"/>
-        <v>LMDSCEMPTY 2802.74725423</v>
+        <v>LMDSCEMPTY 2166.311799883</v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="9"/>
-        <v>LMDSCEMPTY 2793.992921489</v>
+        <v>LMDSCEMPTY 2802.74725423</v>
       </c>
       <c r="AE17" t="str">
         <f t="shared" si="10"/>
+        <v>LMDSCEMPTY 2793.992921489</v>
+      </c>
+      <c r="AH17" t="str">
+        <f t="shared" si="11"/>
         <v>LMDSCEMPTY 2791.724959639</v>
       </c>
     </row>
-    <row r="18" spans="7:31" x14ac:dyDescent="0.25">
-      <c r="G18" t="str">
-        <f t="shared" si="2"/>
-        <v>LMASCEMPTY 2278.39447451</v>
-      </c>
+    <row r="18" spans="10:34" x14ac:dyDescent="0.25">
       <c r="J18" t="str">
         <f t="shared" si="3"/>
-        <v>LMASCEMPTY 2446.22365141</v>
+        <v>LMASCEMPTY 2278.39447451</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="4"/>
-        <v>LMASCEMPTY 2301.573044617</v>
+        <v>LMASCEMPTY 2446.22365141</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="5"/>
-        <v>LMASCEMPTY 2103.30781969</v>
+        <v>LMASCEMPTY 2301.573044617</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="6"/>
-        <v>LMASCEMPTY 2090.425796382</v>
+        <v>LMASCEMPTY 2103.30781969</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="7"/>
-        <v>LMASCEMPTY 2103.30781969</v>
+        <v>LMASCEMPTY 2090.425796382</v>
       </c>
       <c r="Y18" t="str">
         <f t="shared" si="8"/>
-        <v>LMASCEMPTY 2132.473809081</v>
+        <v>LMASCEMPTY 2103.30781969</v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="9"/>
+        <v>LMASCEMPTY 2132.473809081</v>
+      </c>
+      <c r="AE18" t="str">
+        <f t="shared" si="10"/>
         <v>LMASCEMPTY 2141.727093429</v>
       </c>
-      <c r="AE18" t="str">
-        <f>AE9&amp;" "&amp;AF9</f>
+      <c r="AH18" t="str">
+        <f>AH9&amp;" "&amp;AI9</f>
         <v>LMASCEMPTY 2144.675443834</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="P1:Q1"/>
+  <mergeCells count="12">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Apollo 7 masses
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A68A78E-8119-4465-ABB7-6F9BC99E0815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAF7EB7-E1D1-4991-AA7A-CF3FB6AB6002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="18" r:id="rId1"/>
@@ -513,13 +513,13 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2782,7 +2782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72429DAA-B9F6-4DDA-BFC1-E3E1D001C964}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -3986,8 +3986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066B9CA6-04BF-488A-87FF-0D836758BC46}">
   <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,65 +4031,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="10"/>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="22"/>
+      <c r="K1" s="21"/>
       <c r="L1" s="10"/>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="20"/>
+      <c r="N1" s="22"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="22"/>
+      <c r="Q1" s="21"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="20"/>
+      <c r="T1" s="22"/>
       <c r="U1" s="10"/>
-      <c r="V1" s="22" t="s">
+      <c r="V1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="22"/>
+      <c r="W1" s="21"/>
       <c r="X1" s="10"/>
-      <c r="Y1" s="20" t="s">
+      <c r="Y1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="20"/>
+      <c r="Z1" s="22"/>
       <c r="AA1" s="10"/>
-      <c r="AB1" s="22" t="s">
+      <c r="AB1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="22"/>
+      <c r="AC1" s="21"/>
       <c r="AD1" s="10"/>
-      <c r="AE1" s="20" t="s">
+      <c r="AE1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" s="20"/>
+      <c r="AF1" s="22"/>
       <c r="AG1" s="10"/>
-      <c r="AH1" s="22" t="s">
+      <c r="AH1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="AI1" s="22"/>
+      <c r="AI1" s="21"/>
       <c r="AJ1" s="10"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -5170,11 +5170,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
@@ -5182,6 +5177,11 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add titles to other apollo masses
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Spacecraft Masses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC08A5E0-5AAF-4F4B-9DC1-97B1646BE657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A95A3AD-CB5B-46DB-96FF-B5006F396572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="99">
   <si>
     <t>CM Empty Mass</t>
   </si>
@@ -554,20 +554,20 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4032,8 +4032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066B9CA6-04BF-488A-87FF-0D836758BC46}">
   <dimension ref="A1:AJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4077,65 +4077,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="20"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="10"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="21"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="10"/>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="22"/>
+      <c r="N1" s="25"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="21"/>
+      <c r="Q1" s="26"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="22"/>
+      <c r="T1" s="25"/>
       <c r="U1" s="10"/>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="21"/>
+      <c r="W1" s="26"/>
       <c r="X1" s="10"/>
-      <c r="Y1" s="22" t="s">
+      <c r="Y1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="22"/>
+      <c r="Z1" s="25"/>
       <c r="AA1" s="10"/>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="21"/>
+      <c r="AC1" s="26"/>
       <c r="AD1" s="10"/>
-      <c r="AE1" s="22" t="s">
+      <c r="AE1" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" s="22"/>
+      <c r="AF1" s="25"/>
       <c r="AG1" s="10"/>
-      <c r="AH1" s="21" t="s">
+      <c r="AH1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="AI1" s="21"/>
+      <c r="AI1" s="26"/>
       <c r="AJ1" s="10"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -5534,534 +5530,570 @@
       <c r="AJ22" s="12"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="25"/>
       <c r="C23" s="12"/>
+      <c r="D23" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="27"/>
       <c r="F23" s="12"/>
+      <c r="G23" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="25"/>
       <c r="I23" s="12"/>
+      <c r="J23" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K23" s="26"/>
       <c r="L23" s="12"/>
+      <c r="M23" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="N23" s="25"/>
       <c r="O23" s="12"/>
-      <c r="P23" s="21" t="s">
+      <c r="P23" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="Q23" s="21"/>
+      <c r="Q23" s="26"/>
       <c r="R23" s="12"/>
-      <c r="S23" s="22" t="s">
+      <c r="S23" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="T23" s="22"/>
+      <c r="T23" s="25"/>
       <c r="U23" s="12"/>
-      <c r="V23" s="21" t="s">
+      <c r="V23" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="W23" s="21"/>
+      <c r="W23" s="26"/>
       <c r="X23" s="12"/>
-      <c r="Y23" s="22" t="s">
+      <c r="Y23" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="Z23" s="22"/>
+      <c r="Z23" s="25"/>
       <c r="AA23" s="12"/>
-      <c r="AB23" s="21" t="s">
+      <c r="AB23" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="AC23" s="21"/>
+      <c r="AC23" s="26"/>
       <c r="AD23" s="12"/>
-      <c r="AE23" s="22" t="s">
+      <c r="AE23" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="AF23" s="22"/>
+      <c r="AF23" s="25"/>
       <c r="AG23" s="12"/>
-      <c r="AH23" s="21" t="s">
+      <c r="AH23" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="AI23" s="21"/>
-      <c r="AJ23" s="27"/>
+      <c r="AI23" s="26"/>
+      <c r="AJ23" s="24"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="24">
-        <v>0</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="23" t="s">
+      <c r="B24" s="21">
+        <v>0</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="21">
         <f>SUM(E2:E6)</f>
         <v>14885.223291630999</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="23" t="s">
+      <c r="F24" s="24"/>
+      <c r="G24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="21">
         <f>SUM(H2:H6)</f>
         <v>29030.365272370003</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="23" t="s">
+      <c r="I24" s="24"/>
+      <c r="J24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="21">
         <f>SUM(K2:K6)</f>
         <v>26844.957233710003</v>
       </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="23" t="s">
+      <c r="L24" s="24"/>
+      <c r="M24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24" s="21">
         <f>SUM(N2:N6)</f>
         <v>28986.366812480002</v>
       </c>
-      <c r="O24" s="27"/>
-      <c r="P24" s="23" t="s">
+      <c r="O24" s="24"/>
+      <c r="P24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="Q24" s="24">
+      <c r="Q24" s="21">
         <f>SUM(Q2:Q6)</f>
         <v>28952.800977100003</v>
       </c>
-      <c r="R24" s="27"/>
-      <c r="S24" s="23" t="s">
+      <c r="R24" s="24"/>
+      <c r="S24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="T24" s="24">
+      <c r="T24" s="21">
         <f>SUM(T2:T6)</f>
         <v>28932.752194346001</v>
       </c>
-      <c r="U24" s="27"/>
-      <c r="V24" s="23" t="s">
+      <c r="U24" s="24"/>
+      <c r="V24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="W24" s="24">
+      <c r="W24" s="21">
         <f>SUM(W2:W6)</f>
         <v>28880.951945691999</v>
       </c>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="23" t="s">
+      <c r="X24" s="24"/>
+      <c r="Y24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="Z24" s="24">
+      <c r="Z24" s="21">
         <f>SUM(Z2:Z6)</f>
         <v>29323.431302626996</v>
       </c>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="23" t="s">
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AC24" s="24">
+      <c r="AC24" s="21">
         <f>SUM(AC2:AC6)</f>
         <v>30452.195915372002</v>
       </c>
-      <c r="AD24" s="27"/>
-      <c r="AE24" s="23" t="s">
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AF24" s="24">
+      <c r="AF24" s="21">
         <f>SUM(AF2:AF6)</f>
         <v>30416.362118141999</v>
       </c>
-      <c r="AG24" s="27"/>
-      <c r="AH24" s="23" t="s">
+      <c r="AG24" s="24"/>
+      <c r="AH24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AI24" s="24">
+      <c r="AI24" s="21">
         <f>SUM(AI2:AI6)</f>
         <v>30465.985123420003</v>
       </c>
-      <c r="AJ24" s="27"/>
+      <c r="AJ24" s="24"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="25" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="25" t="s">
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="25" t="s">
+      <c r="H25" s="23"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="25" t="s">
+      <c r="K25" s="23"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="N25" s="26"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="25" t="s">
+      <c r="N25" s="23"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="Q25" s="26">
+      <c r="Q25" s="23">
         <v>28751.7</v>
       </c>
-      <c r="R25" s="27"/>
-      <c r="S25" s="25" t="s">
+      <c r="R25" s="24"/>
+      <c r="S25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="T25" s="26">
+      <c r="T25" s="23">
         <v>28792.682870000001</v>
       </c>
-      <c r="U25" s="27"/>
-      <c r="V25" s="25" t="s">
+      <c r="U25" s="24"/>
+      <c r="V25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="W25" s="26">
+      <c r="W25" s="23">
         <v>28883.900300000001</v>
       </c>
-      <c r="X25" s="27"/>
-      <c r="Y25" s="25" t="s">
+      <c r="X25" s="24"/>
+      <c r="Y25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="Z25" s="26">
+      <c r="Z25" s="23">
         <v>29237.25</v>
       </c>
-      <c r="AA25" s="27"/>
-      <c r="AB25" s="25" t="s">
+      <c r="AA25" s="24"/>
+      <c r="AB25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="AC25" s="26">
+      <c r="AC25" s="23">
         <v>30352.224160000002</v>
       </c>
-      <c r="AD25" s="27"/>
-      <c r="AE25" s="25" t="s">
+      <c r="AD25" s="24"/>
+      <c r="AE25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="AF25" s="26">
+      <c r="AF25" s="23">
         <v>30339.705308000001</v>
       </c>
-      <c r="AG25" s="27"/>
-      <c r="AH25" s="25" t="s">
+      <c r="AG25" s="24"/>
+      <c r="AH25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="AI25" s="26">
+      <c r="AI25" s="23">
         <v>30342.33584</v>
       </c>
-      <c r="AJ25" s="27"/>
+      <c r="AJ25" s="24"/>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="21">
         <f>SUM(B2:B6)</f>
         <v>14305.668320482</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="23" t="s">
+      <c r="C26" s="24"/>
+      <c r="D26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="24">
-        <v>0</v>
-      </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="23" t="s">
+      <c r="E26" s="21">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24"/>
+      <c r="G26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="24">
-        <v>0</v>
-      </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="23" t="s">
+      <c r="H26" s="21">
+        <v>0</v>
+      </c>
+      <c r="I26" s="24"/>
+      <c r="J26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="K26" s="24">
+      <c r="K26" s="21">
         <f>SUM(K7:K11)</f>
         <v>14514.955839999999</v>
       </c>
-      <c r="L26" s="27"/>
-      <c r="M26" s="23" t="s">
+      <c r="L26" s="24"/>
+      <c r="M26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="N26" s="24">
+      <c r="N26" s="21">
         <f>SUM(N7:N11)</f>
         <v>14324.310966889001</v>
       </c>
-      <c r="O26" s="27"/>
-      <c r="P26" s="23" t="s">
+      <c r="O26" s="24"/>
+      <c r="P26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="Q26" s="24">
+      <c r="Q26" s="21">
         <f>SUM(Q7:Q11)</f>
         <v>15340.720749585</v>
       </c>
-      <c r="R26" s="27"/>
-      <c r="S26" s="23" t="s">
+      <c r="R26" s="24"/>
+      <c r="S26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="T26" s="24">
+      <c r="T26" s="21">
         <f>SUM(T7:T11)</f>
         <v>15232.765765525002</v>
       </c>
-      <c r="U26" s="27"/>
-      <c r="V26" s="23" t="s">
+      <c r="U26" s="24"/>
+      <c r="V26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="W26" s="24">
+      <c r="W26" s="21">
         <f>SUM(W7:W11)</f>
         <v>15220.428053060999</v>
       </c>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="23" t="s">
+      <c r="X26" s="24"/>
+      <c r="Y26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="Z26" s="24">
+      <c r="Z26" s="21">
         <f>SUM(Z7:Z11)</f>
         <v>15281.209430641002</v>
       </c>
-      <c r="AA26" s="27"/>
-      <c r="AB26" s="23" t="s">
+      <c r="AA26" s="24"/>
+      <c r="AB26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="AC26" s="24">
+      <c r="AC26" s="21">
         <f>SUM(AC7:AC11)</f>
         <v>16469.938954700003</v>
       </c>
-      <c r="AD26" s="27"/>
-      <c r="AE26" s="23" t="s">
+      <c r="AD26" s="24"/>
+      <c r="AE26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="AF26" s="24">
+      <c r="AF26" s="21">
         <f>SUM(AF7:AF11)</f>
         <v>16471.934761128003</v>
       </c>
-      <c r="AG26" s="27"/>
-      <c r="AH26" s="23" t="s">
+      <c r="AG26" s="24"/>
+      <c r="AH26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="AI26" s="24">
+      <c r="AI26" s="21">
         <f>SUM(AI7:AI11)</f>
         <v>16483.546725799999</v>
       </c>
-      <c r="AJ26" s="27"/>
+      <c r="AJ26" s="24"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="25" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="25" t="s">
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="25" t="s">
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="25" t="s">
+      <c r="K27" s="23"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="25" t="s">
+      <c r="N27" s="23"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="Q27" s="26">
+      <c r="Q27" s="23">
         <v>15093.6</v>
       </c>
-      <c r="R27" s="27"/>
-      <c r="S27" s="25" t="s">
+      <c r="R27" s="24"/>
+      <c r="S27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="T27" s="26">
+      <c r="T27" s="23">
         <v>15222.24242</v>
       </c>
-      <c r="U27" s="27"/>
-      <c r="V27" s="25" t="s">
+      <c r="U27" s="24"/>
+      <c r="V27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="W27" s="26">
+      <c r="W27" s="23">
         <v>15159.46524</v>
       </c>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="25" t="s">
+      <c r="X27" s="24"/>
+      <c r="Y27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="Z27" s="26">
+      <c r="Z27" s="23">
         <v>15276.27</v>
       </c>
-      <c r="AA27" s="27"/>
-      <c r="AB27" s="25" t="s">
+      <c r="AA27" s="24"/>
+      <c r="AB27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="AC27" s="26">
+      <c r="AC27" s="23">
         <v>16422.856070000002</v>
       </c>
-      <c r="AD27" s="27"/>
-      <c r="AE27" s="25" t="s">
+      <c r="AD27" s="24"/>
+      <c r="AE27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="AF27" s="26">
+      <c r="AF27" s="23">
         <v>16423.808773000001</v>
       </c>
-      <c r="AG27" s="27"/>
-      <c r="AH27" s="25" t="s">
+      <c r="AG27" s="24"/>
+      <c r="AH27" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="AI27" s="26">
+      <c r="AI27" s="23">
         <v>16445.17281</v>
       </c>
-      <c r="AJ27" s="27"/>
+      <c r="AJ27" s="24"/>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="C28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="X28" s="27"/>
-      <c r="AA28" s="27"/>
-      <c r="AD28" s="27"/>
-      <c r="AG28" s="27"/>
-      <c r="AJ28" s="27"/>
+      <c r="C28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="AA28" s="24"/>
+      <c r="AD28" s="24"/>
+      <c r="AG28" s="24"/>
+      <c r="AJ28" s="24"/>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="C29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="23" t="s">
+      <c r="C29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="Q29" s="24">
+      <c r="Q29" s="21">
         <f>Q24-Q25</f>
         <v>201.10097710000264</v>
       </c>
-      <c r="R29" s="27"/>
-      <c r="S29" s="23" t="s">
+      <c r="R29" s="24"/>
+      <c r="S29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="T29" s="24">
+      <c r="T29" s="21">
         <f>T24-T25</f>
         <v>140.06932434600094</v>
       </c>
-      <c r="U29" s="27"/>
-      <c r="V29" s="23" t="s">
+      <c r="U29" s="24"/>
+      <c r="V29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="W29" s="24">
+      <c r="W29" s="21">
         <f>W24-W25</f>
         <v>-2.9483543080023082</v>
       </c>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="23" t="s">
+      <c r="X29" s="24"/>
+      <c r="Y29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="Z29" s="24">
+      <c r="Z29" s="21">
         <f>Z24-Z25</f>
         <v>86.181302626995603</v>
       </c>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="23" t="s">
+      <c r="AA29" s="24"/>
+      <c r="AB29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="AC29" s="24">
+      <c r="AC29" s="21">
         <f>AC24-AC25</f>
         <v>99.971755372000189</v>
       </c>
-      <c r="AD29" s="27"/>
-      <c r="AE29" s="23" t="s">
+      <c r="AD29" s="24"/>
+      <c r="AE29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="AF29" s="24">
+      <c r="AF29" s="21">
         <f>AF24-AF25</f>
         <v>76.656810141997994</v>
       </c>
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="23" t="s">
+      <c r="AG29" s="24"/>
+      <c r="AH29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="AI29" s="24">
+      <c r="AI29" s="21">
         <f>AI24-AI25</f>
         <v>123.64928342000348</v>
       </c>
-      <c r="AJ29" s="27"/>
+      <c r="AJ29" s="24"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="C30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="23" t="s">
+      <c r="C30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="Q30" s="24">
+      <c r="Q30" s="21">
         <f>Q26-Q27</f>
         <v>247.12074958499943</v>
       </c>
-      <c r="R30" s="27"/>
-      <c r="S30" s="23" t="s">
+      <c r="R30" s="24"/>
+      <c r="S30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="T30" s="24">
+      <c r="T30" s="21">
         <f>T26-T27</f>
         <v>10.523345525001787</v>
       </c>
-      <c r="U30" s="27"/>
-      <c r="V30" s="23" t="s">
+      <c r="U30" s="24"/>
+      <c r="V30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="W30" s="24">
+      <c r="W30" s="21">
         <f>W26-W27</f>
         <v>60.962813060999906</v>
       </c>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="23" t="s">
+      <c r="X30" s="24"/>
+      <c r="Y30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="Z30" s="24">
+      <c r="Z30" s="21">
         <f>Z26-Z27</f>
         <v>4.9394306410013087</v>
       </c>
-      <c r="AA30" s="27"/>
-      <c r="AB30" s="23" t="s">
+      <c r="AA30" s="24"/>
+      <c r="AB30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="AC30" s="24">
+      <c r="AC30" s="21">
         <f>AC26-AC27</f>
         <v>47.082884700001159</v>
       </c>
-      <c r="AD30" s="27"/>
-      <c r="AE30" s="23" t="s">
+      <c r="AD30" s="24"/>
+      <c r="AE30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="AF30" s="24">
+      <c r="AF30" s="21">
         <f>AF26-AF27</f>
         <v>48.125988128002064</v>
       </c>
-      <c r="AG30" s="27"/>
-      <c r="AH30" s="23" t="s">
+      <c r="AG30" s="24"/>
+      <c r="AH30" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="AI30" s="24">
+      <c r="AI30" s="21">
         <f>AI26-AI27</f>
         <v>38.37391579999894</v>
       </c>
-      <c r="AJ30" s="27"/>
+      <c r="AJ30" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="23">
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AH23:AI23"/>
     <mergeCell ref="P23:Q23"/>
@@ -6069,18 +6101,6 @@
     <mergeCell ref="V23:W23"/>
     <mergeCell ref="Y23:Z23"/>
     <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>